<commit_message>
Fixed prefix url for "bev"
Pointing URL to explainer page on Zero Nexus website
</commit_message>
<xml_diff>
--- a/BEV Data Vocabulary.xlsx
+++ b/BEV Data Vocabulary.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://zeronexus.sharepoint.com/sites/EVMO-Glencore/Shared Documents/Glencore/02 BEV Data Taxonomy/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edwar\Github\evmo-vocab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="8_{A6ED6CAB-DBCA-4C40-873E-2F131A62E0B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3D04E05A-2CD9-4E65-BB94-66A5A9B58185}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AE05FD1-D0CB-4570-BCB1-0ADB5CF47F69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{638C754D-6598-4F04-8D33-CB7A05B0560B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{638C754D-6598-4F04-8D33-CB7A05B0560B}"/>
   </bookViews>
   <sheets>
     <sheet name="SKOS" sheetId="3" r:id="rId1"/>
@@ -1175,7 +1175,7 @@
     <t>This spreadsheet contains open definitions for many of the types of data generated by or describing BEVs (battery electric vehicles) and BEV support equipment used in mining.</t>
   </si>
   <si>
-    <t>https://zero.nexus/wp-content/uploads/2025/10/bev.ttl</t>
+    <t>https://zero.nexus/bev-data-vocabulary/</t>
   </si>
 </sst>
 </file>
@@ -1234,7 +1234,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1246,8 +1246,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -1631,7 +1629,7 @@
   <dimension ref="A1:M156"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1652,7 +1650,7 @@
       <c r="A1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="5" t="s">
         <v>343</v>
       </c>
       <c r="G1" s="2"/>
@@ -1663,10 +1661,10 @@
       <c r="A2" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" t="s">
         <v>96</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="5" t="s">
         <v>343</v>
       </c>
       <c r="G2" s="2"/>
@@ -1703,7 +1701,7 @@
       <c r="J5" s="2"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" t="s">
         <v>342</v>
       </c>
       <c r="G6" s="2"/>
@@ -4030,16 +4028,31 @@
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{4DEAB23F-CF01-4AB4-B1E3-CA83451AB1FA}"/>
-    <hyperlink ref="B1" r:id="rId2" xr:uid="{24E73981-1764-4171-AC91-A434CA8A1FF1}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d8e165db-149b-4197-bc76-0f068cbb73e1">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009ECF0953322C9541A9A1EDFD15376FEB" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="be6ec5c2eb01e6dab00300863d7ca40e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d1e4d1e0-c95d-4c51-be4d-468b7a581b67" xmlns:ns3="d8e165db-149b-4197-bc76-0f068cbb73e1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cba18d3b1191ba2ed2ca6b2456b1847e" ns2:_="" ns3:_="">
     <xsd:import namespace="d1e4d1e0-c95d-4c51-be4d-468b7a581b67"/>
@@ -4250,26 +4263,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0058CAD2-89AE-44C8-AF19-A0D04C3633AC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="d8e165db-149b-4197-bc76-0f068cbb73e1"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d8e165db-149b-4197-bc76-0f068cbb73e1">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B902C61F-C425-480E-9AE8-5743FFC97C42}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4BFD419B-CB92-44D3-B027-0EE3D3BB0D32}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4286,22 +4298,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B902C61F-C425-480E-9AE8-5743FFC97C42}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0058CAD2-89AE-44C8-AF19-A0D04C3633AC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="d8e165db-149b-4197-bc76-0f068cbb73e1"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fixed typo with "Charge Connector" entity
</commit_message>
<xml_diff>
--- a/BEV Data Vocabulary.xlsx
+++ b/BEV Data Vocabulary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edwar\Github\evmo-vocab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AE05FD1-D0CB-4570-BCB1-0ADB5CF47F69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B452B17-280A-491C-B660-15EE760125CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{638C754D-6598-4F04-8D33-CB7A05B0560B}"/>
   </bookViews>
@@ -266,9 +266,6 @@
     <t>Max Charge Rate</t>
   </si>
   <si>
-    <t>Charge Connector</t>
-  </si>
-  <si>
     <t>Year manufactured</t>
   </si>
   <si>
@@ -1176,6 +1173,9 @@
   </si>
   <si>
     <t>https://zero.nexus/bev-data-vocabulary/</t>
+  </si>
+  <si>
+    <t>Charge Connector</t>
   </si>
 </sst>
 </file>
@@ -1628,8 +1628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CA4D3C4-3E4D-4807-81BB-CD57E0DDC2A2}">
   <dimension ref="A1:M156"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1648,10 +1648,10 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="G1" s="2"/>
       <c r="I1" s="2"/>
@@ -1659,13 +1659,13 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="G2" s="2"/>
       <c r="I2" s="2"/>
@@ -1673,10 +1673,10 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C3" s="2"/>
       <c r="G3" s="2"/>
@@ -1685,10 +1685,10 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C4" s="2"/>
       <c r="G4" s="2"/>
@@ -1702,7 +1702,7 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G6" s="2"/>
       <c r="I6" s="2"/>
@@ -1720,43 +1720,43 @@
     </row>
     <row r="9" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="E9" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="F9" s="4" t="s">
+      <c r="G9" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="I9" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="G9" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="H9" s="4" t="s">
+      <c r="J9" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="M9" s="3" t="s">
         <v>106</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="J9" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="K9" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="L9" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="M9" s="3" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -1765,13 +1765,13 @@
         <v>bev:vehicle_data</v>
       </c>
       <c r="B10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C10" t="s">
         <v>0</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -1780,13 +1780,13 @@
         <v>bev:battery_data</v>
       </c>
       <c r="B11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -1795,13 +1795,13 @@
         <v>bev:charger_data</v>
       </c>
       <c r="B12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -1810,13 +1810,13 @@
         <v>bev:facility_data</v>
       </c>
       <c r="B13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C13" t="s">
         <v>3</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -1825,13 +1825,13 @@
         <v>bev:maintenance_data</v>
       </c>
       <c r="B14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C14" t="s">
         <v>2</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -1840,13 +1840,13 @@
         <v>bev:production_data</v>
       </c>
       <c r="B15" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C15" t="s">
+        <v>174</v>
+      </c>
+      <c r="F15" s="2" t="s">
         <v>175</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -1855,13 +1855,13 @@
         <v>bev:availability_kpis</v>
       </c>
       <c r="B16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C16" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1870,13 +1870,13 @@
         <v>bev:utilization_kpis</v>
       </c>
       <c r="B17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C17" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1885,13 +1885,13 @@
         <v>bev:effectiveness_kpis</v>
       </c>
       <c r="B18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C18" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1900,13 +1900,13 @@
         <v>bev:maintenance_kpis</v>
       </c>
       <c r="B19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C19" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1918,10 +1918,10 @@
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -1933,10 +1933,10 @@
         <v>12</v>
       </c>
       <c r="E21" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -1948,10 +1948,10 @@
         <v>27</v>
       </c>
       <c r="E22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1963,10 +1963,10 @@
         <v>28</v>
       </c>
       <c r="E23" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -1978,10 +1978,10 @@
         <v>29</v>
       </c>
       <c r="E24" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1990,13 +1990,13 @@
         <v>bev:rebuild_count</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E25" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -2005,13 +2005,13 @@
         <v>bev:last_rebuild_year</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E26" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2023,10 +2023,10 @@
         <v>30</v>
       </c>
       <c r="E27" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -2038,10 +2038,10 @@
         <v>31</v>
       </c>
       <c r="E28" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2050,13 +2050,13 @@
         <v>bev:functional_location</v>
       </c>
       <c r="C29" t="s">
+        <v>327</v>
+      </c>
+      <c r="E29" t="s">
+        <v>237</v>
+      </c>
+      <c r="F29" s="2" t="s">
         <v>328</v>
-      </c>
-      <c r="E29" t="s">
-        <v>238</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -2065,16 +2065,16 @@
         <v>bev:energy_system_architecture</v>
       </c>
       <c r="C30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E30" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2083,16 +2083,16 @@
         <v>bev:vehicle_type</v>
       </c>
       <c r="C31" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E31" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2101,16 +2101,16 @@
         <v>bev:vehicle_class</v>
       </c>
       <c r="C32" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E32" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -2119,16 +2119,16 @@
         <v>bev:vehicle_function</v>
       </c>
       <c r="C33" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E33" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -2140,10 +2140,10 @@
         <v>32</v>
       </c>
       <c r="E34" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -2152,16 +2152,16 @@
         <v>bev:gross_vehicle_weight</v>
       </c>
       <c r="C35" t="s">
+        <v>134</v>
+      </c>
+      <c r="E35" t="s">
+        <v>108</v>
+      </c>
+      <c r="F35" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="E35" t="s">
-        <v>109</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>136</v>
-      </c>
       <c r="K35" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
@@ -2170,13 +2170,13 @@
         <v>bev:purchase_cost</v>
       </c>
       <c r="C36" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E36" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -2188,10 +2188,10 @@
         <v>33</v>
       </c>
       <c r="E37" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -2203,10 +2203,10 @@
         <v>34</v>
       </c>
       <c r="E38" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -2218,10 +2218,10 @@
         <v>35</v>
       </c>
       <c r="E39" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
@@ -2233,10 +2233,10 @@
         <v>36</v>
       </c>
       <c r="E40" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -2245,16 +2245,16 @@
         <v>bev:auxiliary_powered_heater</v>
       </c>
       <c r="C41" t="s">
+        <v>107</v>
+      </c>
+      <c r="E41" t="s">
         <v>108</v>
       </c>
-      <c r="E41" t="s">
-        <v>109</v>
-      </c>
       <c r="F41" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="H41" s="2" t="s">
         <v>334</v>
-      </c>
-      <c r="H41" s="2" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -2266,28 +2266,28 @@
         <v>39</v>
       </c>
       <c r="E42" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="43" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" t="str">
-        <f t="shared" si="1"/>
-        <v>bev:charge connector</v>
+        <f>CONCATENATE("bev:",LOWER(SUBSTITUTE(C43, " ", "_")))</f>
+        <v>bev:charge_connector</v>
       </c>
       <c r="C43" t="s">
-        <v>40</v>
+        <v>343</v>
       </c>
       <c r="E43" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -2296,13 +2296,13 @@
         <v>bev:measurement_start</v>
       </c>
       <c r="C44" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E44" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="45" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -2311,13 +2311,13 @@
         <v>bev:measurement_end</v>
       </c>
       <c r="C45" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E45" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="46" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -2326,13 +2326,13 @@
         <v>bev:vehicle_hours</v>
       </c>
       <c r="C46" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E46" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="47" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -2344,10 +2344,10 @@
         <v>11</v>
       </c>
       <c r="E47" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
@@ -2356,13 +2356,13 @@
         <v>bev:vehicle_idling_time</v>
       </c>
       <c r="C48" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E48" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -2374,10 +2374,10 @@
         <v>4</v>
       </c>
       <c r="E49" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -2389,10 +2389,10 @@
         <v>5</v>
       </c>
       <c r="E50" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -2401,13 +2401,13 @@
         <v>bev:queue_time</v>
       </c>
       <c r="C51" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E51" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -2416,13 +2416,13 @@
         <v>bev:battery_swapping_time</v>
       </c>
       <c r="C52" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E52" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -2431,13 +2431,13 @@
         <v>bev:start_location</v>
       </c>
       <c r="C53" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E53" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -2446,13 +2446,13 @@
         <v>bev:end_location</v>
       </c>
       <c r="C54" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E54" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2461,13 +2461,13 @@
         <v>bev:location</v>
       </c>
       <c r="C55" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E55" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2479,10 +2479,10 @@
         <v>20</v>
       </c>
       <c r="E56" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
@@ -2491,13 +2491,13 @@
         <v>bev:speed</v>
       </c>
       <c r="C57" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E57" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -2506,13 +2506,13 @@
         <v>bev:acceleration</v>
       </c>
       <c r="C58" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E58" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2521,13 +2521,13 @@
         <v>bev:number_of_charging_sessions</v>
       </c>
       <c r="C59" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E59" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2539,10 +2539,10 @@
         <v>16</v>
       </c>
       <c r="E60" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2554,10 +2554,10 @@
         <v>9</v>
       </c>
       <c r="E61" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2569,10 +2569,10 @@
         <v>10</v>
       </c>
       <c r="E62" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
@@ -2584,10 +2584,10 @@
         <v>19</v>
       </c>
       <c r="E63" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
@@ -2596,13 +2596,13 @@
         <v>bev:hydraulic_system_energy</v>
       </c>
       <c r="C64" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E64" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="65" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2611,13 +2611,13 @@
         <v>bev:hydraulic_system_power</v>
       </c>
       <c r="C65" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E65" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="66" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2629,10 +2629,10 @@
         <v>17</v>
       </c>
       <c r="E66" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="67" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2644,10 +2644,10 @@
         <v>18</v>
       </c>
       <c r="E67" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
@@ -2656,13 +2656,13 @@
         <v>bev:payload</v>
       </c>
       <c r="C68" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E68" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="69" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2671,13 +2671,13 @@
         <v>bev:inclination</v>
       </c>
       <c r="C69" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E69" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
@@ -2686,13 +2686,13 @@
         <v>bev:alert_id</v>
       </c>
       <c r="C70" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E70" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
@@ -2701,13 +2701,13 @@
         <v>bev:alert_type</v>
       </c>
       <c r="C71" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E71" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
@@ -2716,13 +2716,13 @@
         <v>bev:alert_description</v>
       </c>
       <c r="C72" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E72" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
@@ -2731,13 +2731,13 @@
         <v>bev:alert_date_time</v>
       </c>
       <c r="C73" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E73" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
@@ -2746,13 +2746,13 @@
         <v>bev:alert_status</v>
       </c>
       <c r="C74" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E74" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
@@ -2764,10 +2764,10 @@
         <v>12</v>
       </c>
       <c r="E75" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="76" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2776,13 +2776,13 @@
         <v>bev:pack_id</v>
       </c>
       <c r="C76" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E76" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
@@ -2794,10 +2794,10 @@
         <v>23</v>
       </c>
       <c r="E77" t="s">
+        <v>202</v>
+      </c>
+      <c r="F77" s="2" t="s">
         <v>203</v>
-      </c>
-      <c r="F77" s="2" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
@@ -2806,13 +2806,13 @@
         <v>bev:cell_id</v>
       </c>
       <c r="C78" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E78" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
@@ -2824,13 +2824,13 @@
         <v>37</v>
       </c>
       <c r="E79" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H79" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
@@ -2842,10 +2842,10 @@
         <v>31</v>
       </c>
       <c r="E80" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
@@ -2854,13 +2854,13 @@
         <v>bev:number_of_cells</v>
       </c>
       <c r="C81" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E81" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
@@ -2869,13 +2869,13 @@
         <v>bev:number_of_modules</v>
       </c>
       <c r="C82" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E82" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="83" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -2884,13 +2884,13 @@
         <v>bev:number_of_packs</v>
       </c>
       <c r="C83" t="s">
+        <v>212</v>
+      </c>
+      <c r="E83" t="s">
+        <v>202</v>
+      </c>
+      <c r="F83" s="2" t="s">
         <v>213</v>
-      </c>
-      <c r="E83" t="s">
-        <v>203</v>
-      </c>
-      <c r="F83" s="2" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
@@ -2902,10 +2902,10 @@
         <v>38</v>
       </c>
       <c r="E84" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
@@ -2914,13 +2914,13 @@
         <v>bev:model</v>
       </c>
       <c r="C85" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E85" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.25">
@@ -2929,13 +2929,13 @@
         <v>bev:battery_mass</v>
       </c>
       <c r="C86" t="s">
+        <v>250</v>
+      </c>
+      <c r="E86" t="s">
+        <v>202</v>
+      </c>
+      <c r="F86" s="2" t="s">
         <v>251</v>
-      </c>
-      <c r="E86" t="s">
-        <v>203</v>
-      </c>
-      <c r="F86" s="2" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="87" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -2947,10 +2947,10 @@
         <v>6</v>
       </c>
       <c r="E87" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="88" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -2962,10 +2962,10 @@
         <v>7</v>
       </c>
       <c r="E88" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="89" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -2974,16 +2974,16 @@
         <v>bev:soc</v>
       </c>
       <c r="C89" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E89" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="K89" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="90" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -2995,10 +2995,10 @@
         <v>8</v>
       </c>
       <c r="E90" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="91" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -3007,13 +3007,13 @@
         <v>bev:energy_consumption</v>
       </c>
       <c r="C91" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E91" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="92" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -3022,13 +3022,13 @@
         <v>bev:regen_energy_generation</v>
       </c>
       <c r="C92" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E92" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="93" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -3037,13 +3037,13 @@
         <v>bev:net_energy_consumption</v>
       </c>
       <c r="C93" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E93" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="94" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -3055,10 +3055,10 @@
         <v>21</v>
       </c>
       <c r="E94" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="95" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -3070,10 +3070,10 @@
         <v>22</v>
       </c>
       <c r="E95" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.25">
@@ -3085,10 +3085,10 @@
         <v>24</v>
       </c>
       <c r="E96" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.25">
@@ -3100,10 +3100,10 @@
         <v>25</v>
       </c>
       <c r="E97" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.25">
@@ -3115,10 +3115,10 @@
         <v>26</v>
       </c>
       <c r="E98" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F98" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.25">
@@ -3127,13 +3127,13 @@
         <v>bev:battery_temperature</v>
       </c>
       <c r="C99" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E99" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F99" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="100" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -3142,16 +3142,16 @@
         <v>bev:soh</v>
       </c>
       <c r="C100" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E100" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="K100" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.25">
@@ -3160,13 +3160,13 @@
         <v>bev:charger_id</v>
       </c>
       <c r="C101" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E101" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F101" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.25">
@@ -3175,13 +3175,13 @@
         <v>bev:connector_id</v>
       </c>
       <c r="C102" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E102" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F102" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="103" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -3190,13 +3190,13 @@
         <v>bev:max_power</v>
       </c>
       <c r="C103" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E103" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F103" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.25">
@@ -3205,13 +3205,13 @@
         <v>bev:rated_power</v>
       </c>
       <c r="C104" t="s">
+        <v>243</v>
+      </c>
+      <c r="E104" t="s">
+        <v>233</v>
+      </c>
+      <c r="F104" s="2" t="s">
         <v>244</v>
-      </c>
-      <c r="E104" t="s">
-        <v>234</v>
-      </c>
-      <c r="F104" s="2" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="105" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -3220,13 +3220,13 @@
         <v>bev:charger_location</v>
       </c>
       <c r="C105" t="s">
+        <v>247</v>
+      </c>
+      <c r="E105" t="s">
+        <v>233</v>
+      </c>
+      <c r="F105" s="2" t="s">
         <v>248</v>
-      </c>
-      <c r="E105" t="s">
-        <v>234</v>
-      </c>
-      <c r="F105" s="2" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="106" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -3235,13 +3235,13 @@
         <v>bev:charge_start_time</v>
       </c>
       <c r="C106" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E106" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="107" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -3250,13 +3250,13 @@
         <v>bev:charge_end_time</v>
       </c>
       <c r="C107" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E107" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.25">
@@ -3265,13 +3265,13 @@
         <v>bev:charging_time</v>
       </c>
       <c r="C108" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E108" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F108" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="109" spans="1:11" x14ac:dyDescent="0.25">
@@ -3280,13 +3280,13 @@
         <v>bev:charging_power</v>
       </c>
       <c r="C109" t="s">
+        <v>240</v>
+      </c>
+      <c r="E109" t="s">
+        <v>233</v>
+      </c>
+      <c r="F109" s="2" t="s">
         <v>241</v>
-      </c>
-      <c r="E109" t="s">
-        <v>234</v>
-      </c>
-      <c r="F109" s="2" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="110" spans="1:11" x14ac:dyDescent="0.25">
@@ -3295,19 +3295,19 @@
         <v>bev:charging_rate</v>
       </c>
       <c r="C110" t="s">
+        <v>324</v>
+      </c>
+      <c r="E110" t="s">
+        <v>233</v>
+      </c>
+      <c r="F110" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="H110" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="K110" t="s">
         <v>325</v>
-      </c>
-      <c r="E110" t="s">
-        <v>234</v>
-      </c>
-      <c r="F110" s="2" t="s">
-        <v>340</v>
-      </c>
-      <c r="H110" s="2" t="s">
-        <v>339</v>
-      </c>
-      <c r="K110" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="111" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -3316,13 +3316,13 @@
         <v>bev:total_energy_delivered</v>
       </c>
       <c r="C111" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E111" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F111" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="112" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -3331,13 +3331,13 @@
         <v>bev:work_order_id</v>
       </c>
       <c r="C112" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E112" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F112" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="113" spans="1:11" x14ac:dyDescent="0.25">
@@ -3346,13 +3346,13 @@
         <v>bev:work_order_description</v>
       </c>
       <c r="C113" t="s">
+        <v>256</v>
+      </c>
+      <c r="E113" t="s">
+        <v>249</v>
+      </c>
+      <c r="F113" s="2" t="s">
         <v>257</v>
-      </c>
-      <c r="E113" t="s">
-        <v>250</v>
-      </c>
-      <c r="F113" s="2" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="114" spans="1:11" x14ac:dyDescent="0.25">
@@ -3361,13 +3361,13 @@
         <v>bev:work_order_status</v>
       </c>
       <c r="C114" t="s">
+        <v>258</v>
+      </c>
+      <c r="E114" t="s">
+        <v>249</v>
+      </c>
+      <c r="F114" s="2" t="s">
         <v>259</v>
-      </c>
-      <c r="E114" t="s">
-        <v>250</v>
-      </c>
-      <c r="F114" s="2" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="115" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -3376,13 +3376,13 @@
         <v>bev:technician_name</v>
       </c>
       <c r="C115" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E115" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F115" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="116" spans="1:11" x14ac:dyDescent="0.25">
@@ -3391,13 +3391,13 @@
         <v>bev:work_order_type</v>
       </c>
       <c r="C116" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E116" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F116" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="117" spans="1:11" x14ac:dyDescent="0.25">
@@ -3406,13 +3406,13 @@
         <v>bev:priority</v>
       </c>
       <c r="C117" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E117" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F117" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="118" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -3421,13 +3421,13 @@
         <v>bev:work_center</v>
       </c>
       <c r="C118" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E118" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F118" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="119" spans="1:11" x14ac:dyDescent="0.25">
@@ -3436,13 +3436,13 @@
         <v>bev:work_order_start</v>
       </c>
       <c r="C119" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E119" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F119" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="120" spans="1:11" x14ac:dyDescent="0.25">
@@ -3451,13 +3451,13 @@
         <v>bev:work_order_end</v>
       </c>
       <c r="C120" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E120" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F120" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="121" spans="1:11" x14ac:dyDescent="0.25">
@@ -3466,13 +3466,13 @@
         <v>bev:total_costs</v>
       </c>
       <c r="C121" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E121" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F121" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="122" spans="1:11" x14ac:dyDescent="0.25">
@@ -3481,13 +3481,13 @@
         <v>bev:part_costs</v>
       </c>
       <c r="C122" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E122" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F122" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="123" spans="1:11" x14ac:dyDescent="0.25">
@@ -3496,13 +3496,13 @@
         <v>bev:labour_costs</v>
       </c>
       <c r="C123" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E123" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F123" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="124" spans="1:11" x14ac:dyDescent="0.25">
@@ -3511,13 +3511,13 @@
         <v>bev:time_in_workshop</v>
       </c>
       <c r="C124" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E124" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F124" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="125" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -3526,13 +3526,13 @@
         <v>bev:logistic_delay</v>
       </c>
       <c r="C125" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E125" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F125" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="126" spans="1:11" x14ac:dyDescent="0.25">
@@ -3541,16 +3541,16 @@
         <v>bev:time_to_repair</v>
       </c>
       <c r="C126" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E126" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F126" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="K126" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="127" spans="1:11" x14ac:dyDescent="0.25">
@@ -3559,13 +3559,13 @@
         <v>bev:idle_time</v>
       </c>
       <c r="C127" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E127" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F127" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="128" spans="1:11" x14ac:dyDescent="0.25">
@@ -3574,13 +3574,13 @@
         <v>bev:mean_time_to_repair</v>
       </c>
       <c r="C128" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E128" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F128" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="K128" t="s">
         <v>13</v>
@@ -3592,13 +3592,13 @@
         <v>bev:mean_time_between_failures</v>
       </c>
       <c r="C129" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E129" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F129" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="K129" t="s">
         <v>14</v>
@@ -3610,13 +3610,13 @@
         <v>bev:mean_time_between_maintenance</v>
       </c>
       <c r="C130" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E130" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F130" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K130" t="s">
         <v>15</v>
@@ -3628,16 +3628,16 @@
         <v>bev:mean_down_time</v>
       </c>
       <c r="C131" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E131" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F131" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="K131" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="132" spans="1:11" x14ac:dyDescent="0.25">
@@ -3646,13 +3646,13 @@
         <v>bev:calendar_time</v>
       </c>
       <c r="C132" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E132" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F132" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="133" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -3661,13 +3661,13 @@
         <v>bev:scheduled_time</v>
       </c>
       <c r="C133" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E133" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F133" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="134" spans="1:11" x14ac:dyDescent="0.25">
@@ -3676,13 +3676,13 @@
         <v>bev:unscheduled_time</v>
       </c>
       <c r="C134" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E134" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F134" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="135" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -3691,16 +3691,16 @@
         <v>bev:down_time</v>
       </c>
       <c r="C135" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E135" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F135" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="K135" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="136" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -3709,13 +3709,13 @@
         <v>bev:available_time</v>
       </c>
       <c r="C136" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E136" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F136" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="137" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -3724,13 +3724,13 @@
         <v>bev:standby_time</v>
       </c>
       <c r="C137" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E137" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F137" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="138" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -3739,13 +3739,13 @@
         <v>bev:operating_standby_time</v>
       </c>
       <c r="C138" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E138" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F138" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="139" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -3754,13 +3754,13 @@
         <v>bev:external_standby_time</v>
       </c>
       <c r="C139" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E139" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F139" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="140" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -3769,13 +3769,13 @@
         <v>bev:operating_time</v>
       </c>
       <c r="C140" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E140" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F140" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="141" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -3784,13 +3784,13 @@
         <v>bev:operating_delay</v>
       </c>
       <c r="C141" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E141" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F141" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="142" spans="1:11" ht="75" x14ac:dyDescent="0.25">
@@ -3799,13 +3799,13 @@
         <v>bev:working_time</v>
       </c>
       <c r="C142" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E142" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F142" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="143" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -3814,13 +3814,13 @@
         <v>bev:non-productive_time</v>
       </c>
       <c r="C143" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E143" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F143" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="144" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -3829,13 +3829,13 @@
         <v>bev:productive_time</v>
       </c>
       <c r="C144" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E144" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F144" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="145" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -3844,16 +3844,16 @@
         <v>bev:up_time</v>
       </c>
       <c r="C145" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E145" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F145" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="K145" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="146" spans="1:11" ht="75" x14ac:dyDescent="0.25">
@@ -3862,13 +3862,13 @@
         <v>bev:availability</v>
       </c>
       <c r="C146" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E146" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F146" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="147" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -3877,13 +3877,13 @@
         <v>bev:physical_availability</v>
       </c>
       <c r="C147" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E147" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F147" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="148" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -3892,13 +3892,13 @@
         <v>bev:mechanical_availability</v>
       </c>
       <c r="C148" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E148" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F148" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="149" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -3907,13 +3907,13 @@
         <v>bev:use_of_availability</v>
       </c>
       <c r="C149" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E149" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F149" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="150" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -3922,13 +3922,13 @@
         <v>bev:asset_utilization</v>
       </c>
       <c r="C150" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E150" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F150" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="151" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -3937,13 +3937,13 @@
         <v>bev:operating_utilization</v>
       </c>
       <c r="C151" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E151" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F151" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="152" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -3952,13 +3952,13 @@
         <v>bev:effective_utilization</v>
       </c>
       <c r="C152" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E152" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F152" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="153" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -3967,13 +3967,13 @@
         <v>bev:operating_efficiency</v>
       </c>
       <c r="C153" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E153" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F153" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="154" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -3982,13 +3982,13 @@
         <v>bev:production_effectiveness</v>
       </c>
       <c r="C154" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E154" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F154" s="2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="155" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -3997,16 +3997,16 @@
         <v>bev:overall_equipment_effectiveness</v>
       </c>
       <c r="C155" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E155" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F155" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="K155" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="156" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -4015,16 +4015,16 @@
         <v>bev:mean_operating_time</v>
       </c>
       <c r="C156" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E156" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F156" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="K156" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -4034,25 +4034,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d8e165db-149b-4197-bc76-0f068cbb73e1">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009ECF0953322C9541A9A1EDFD15376FEB" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="be6ec5c2eb01e6dab00300863d7ca40e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d1e4d1e0-c95d-4c51-be4d-468b7a581b67" xmlns:ns3="d8e165db-149b-4197-bc76-0f068cbb73e1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cba18d3b1191ba2ed2ca6b2456b1847e" ns2:_="" ns3:_="">
     <xsd:import namespace="d1e4d1e0-c95d-4c51-be4d-468b7a581b67"/>
@@ -4263,25 +4244,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0058CAD2-89AE-44C8-AF19-A0D04C3633AC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="d8e165db-149b-4197-bc76-0f068cbb73e1"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B902C61F-C425-480E-9AE8-5743FFC97C42}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d8e165db-149b-4197-bc76-0f068cbb73e1">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4BFD419B-CB92-44D3-B027-0EE3D3BB0D32}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4298,4 +4280,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B902C61F-C425-480E-9AE8-5743FFC97C42}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0058CAD2-89AE-44C8-AF19-A0D04C3633AC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="d8e165db-149b-4197-bc76-0f068cbb73e1"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Replacing SKOS collections with "broader" concept
</commit_message>
<xml_diff>
--- a/BEV Data Vocabulary.xlsx
+++ b/BEV Data Vocabulary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edwar\Github\evmo-vocab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B452B17-280A-491C-B660-15EE760125CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5280F41E-ECE8-476B-86AD-AADC2D3D9DCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{638C754D-6598-4F04-8D33-CB7A05B0560B}"/>
   </bookViews>
@@ -45,7 +45,6 @@
     <author>tc={A618E68F-8989-4945-8237-5E2E94204399}</author>
     <author>tc={68F19B4E-3CDF-4D76-98DC-5E1D1661D124}</author>
     <author>tc={A5299D7F-EF6A-41E1-86D7-CD54D12BD6E5}</author>
-    <author>tc={F5EEE7A5-5DB0-4ADE-869D-EB475B7A632D}</author>
     <author>tc={4F677B91-F839-4803-821F-863632CEE9C7}</author>
     <author>tc={E3BAE7AF-06FD-4F29-A519-CC01008255BD}</author>
     <author>tc={7EA8BFEA-4870-4DA4-8522-C139F2E054EB}</author>
@@ -107,15 +106,7 @@
     Concept is narrower than</t>
       </text>
     </comment>
-    <comment ref="J9" authorId="7" shapeId="0" xr:uid="{F5EEE7A5-5DB0-4ADE-869D-EB475B7A632D}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Concept is broader than</t>
-      </text>
-    </comment>
-    <comment ref="K9" authorId="8" shapeId="0" xr:uid="{4F677B91-F839-4803-821F-863632CEE9C7}">
+    <comment ref="K9" authorId="7" shapeId="0" xr:uid="{4F677B91-F839-4803-821F-863632CEE9C7}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -123,7 +114,7 @@
     Simplified notational form</t>
       </text>
     </comment>
-    <comment ref="L9" authorId="9" shapeId="0" xr:uid="{E3BAE7AF-06FD-4F29-A519-CC01008255BD}">
+    <comment ref="L9" authorId="8" shapeId="0" xr:uid="{E3BAE7AF-06FD-4F29-A519-CC01008255BD}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -131,7 +122,7 @@
     Editorial note for developing concept scheme</t>
       </text>
     </comment>
-    <comment ref="M9" authorId="10" shapeId="0" xr:uid="{7EA8BFEA-4870-4DA4-8522-C139F2E054EB}">
+    <comment ref="M9" authorId="9" shapeId="0" xr:uid="{7EA8BFEA-4870-4DA4-8522-C139F2E054EB}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -144,7 +135,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="343">
   <si>
     <t>Vehicle Data</t>
   </si>
@@ -455,9 +446,6 @@
     <t>dct:description@en</t>
   </si>
   <si>
-    <t>skos:broader@en</t>
-  </si>
-  <si>
     <t>skos:scopeNote@en</t>
   </si>
   <si>
@@ -497,9 +485,6 @@
     <t>^skos:member</t>
   </si>
   <si>
-    <t>skos:Collection</t>
-  </si>
-  <si>
     <t>Work Order ID</t>
   </si>
   <si>
@@ -512,9 +497,6 @@
     <t>Description of BEV and BEV support equipment data types</t>
   </si>
   <si>
-    <t>bev:vehicle_data, bev:battery_data</t>
-  </si>
-  <si>
     <t>All data relating to the description and use of a battery electric vehicle (BEV)</t>
   </si>
   <si>
@@ -857,9 +839,6 @@
     <t>The ID number for the connector</t>
   </si>
   <si>
-    <t>bev:vehicle_data, bev:battery_data, bev:charger_data</t>
-  </si>
-  <si>
     <t>The start date/time of a charging session</t>
   </si>
   <si>
@@ -1067,18 +1046,6 @@
     <t>Key Performance Indicators (KPIs) relating to equipment maintenance</t>
   </si>
   <si>
-    <t>bev:production_data, bev:availability_kpis</t>
-  </si>
-  <si>
-    <t>bev:production_data, bev:utilization_kpis</t>
-  </si>
-  <si>
-    <t>bev:production_data, bev:effectiveness_kpis</t>
-  </si>
-  <si>
-    <t>bev:maintenance_data, bev:maintenance_kpis</t>
-  </si>
-  <si>
     <t>The time the equipment is operated as a percentage of the available time</t>
   </si>
   <si>
@@ -1176,6 +1143,27 @@
   </si>
   <si>
     <t>Charge Connector</t>
+  </si>
+  <si>
+    <t>bev:vehicle_data,bev:battery_data</t>
+  </si>
+  <si>
+    <t>bev:vehicle_data,bev:battery_data,bev:charger_data</t>
+  </si>
+  <si>
+    <t>bev:maintenance_data,bev:maintenance_kpis</t>
+  </si>
+  <si>
+    <t>bev:production_data,bev:availability_kpis</t>
+  </si>
+  <si>
+    <t>bev:production_data,bev:utilization_kpis</t>
+  </si>
+  <si>
+    <t>bev:production_data,bev:effectiveness_kpis</t>
+  </si>
+  <si>
+    <t>skos:broader(separator=",")</t>
   </si>
 </sst>
 </file>
@@ -1609,9 +1597,6 @@
   <threadedComment ref="I9" dT="2025-01-08T22:25:41.67" personId="{D8C6BBBD-B858-4E95-8943-91C985B8D7D2}" id="{A5299D7F-EF6A-41E1-86D7-CD54D12BD6E5}">
     <text>Concept is narrower than</text>
   </threadedComment>
-  <threadedComment ref="J9" dT="2025-01-08T22:25:41.67" personId="{D8C6BBBD-B858-4E95-8943-91C985B8D7D2}" id="{F5EEE7A5-5DB0-4ADE-869D-EB475B7A632D}">
-    <text>Concept is broader than</text>
-  </threadedComment>
   <threadedComment ref="K9" dT="2025-01-08T22:26:20.33" personId="{D8C6BBBD-B858-4E95-8943-91C985B8D7D2}" id="{4F677B91-F839-4803-821F-863632CEE9C7}">
     <text>Simplified notational form</text>
   </threadedComment>
@@ -1628,8 +1613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CA4D3C4-3E4D-4807-81BB-CD57E0DDC2A2}">
   <dimension ref="A1:M156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1642,7 +1627,9 @@
     <col min="6" max="6" width="33" style="2" customWidth="1"/>
     <col min="7" max="7" width="28" customWidth="1"/>
     <col min="8" max="8" width="28" style="2" customWidth="1"/>
-    <col min="9" max="12" width="28" customWidth="1"/>
+    <col min="9" max="9" width="28" customWidth="1"/>
+    <col min="10" max="10" width="48.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="28" customWidth="1"/>
     <col min="13" max="13" width="30" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1651,7 +1638,7 @@
         <v>91</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="G1" s="2"/>
       <c r="I1" s="2"/>
@@ -1665,7 +1652,7 @@
         <v>95</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="G2" s="2"/>
       <c r="I2" s="2"/>
@@ -1688,7 +1675,7 @@
         <v>102</v>
       </c>
       <c r="B4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C4" s="2"/>
       <c r="G4" s="2"/>
@@ -1702,7 +1689,7 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>341</v>
+        <v>333</v>
       </c>
       <c r="G6" s="2"/>
       <c r="I6" s="2"/>
@@ -1718,36 +1705,36 @@
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
     </row>
-    <row r="9" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>93</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>96</v>
       </c>
       <c r="D9" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>115</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>116</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>97</v>
       </c>
       <c r="G9" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="H9" s="4" t="s">
         <v>104</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>105</v>
       </c>
       <c r="I9" s="4" t="s">
         <v>98</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>103</v>
+        <v>342</v>
       </c>
       <c r="K9" s="3" t="s">
         <v>99</v>
@@ -1756,7 +1743,7 @@
         <v>100</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -1764,14 +1751,11 @@
         <f t="shared" ref="A10:A19" si="0">CONCATENATE("bev:",LOWER(SUBSTITUTE(C10, " ", "_")))</f>
         <v>bev:vehicle_data</v>
       </c>
-      <c r="B10" t="s">
-        <v>117</v>
-      </c>
       <c r="C10" t="s">
         <v>0</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -1779,14 +1763,11 @@
         <f t="shared" si="0"/>
         <v>bev:battery_data</v>
       </c>
-      <c r="B11" t="s">
-        <v>117</v>
-      </c>
       <c r="C11" t="s">
         <v>74</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -1794,14 +1775,11 @@
         <f t="shared" si="0"/>
         <v>bev:charger_data</v>
       </c>
-      <c r="B12" t="s">
-        <v>117</v>
-      </c>
       <c r="C12" t="s">
         <v>45</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -1809,14 +1787,11 @@
         <f t="shared" si="0"/>
         <v>bev:facility_data</v>
       </c>
-      <c r="B13" t="s">
-        <v>117</v>
-      </c>
       <c r="C13" t="s">
         <v>3</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -1824,14 +1799,11 @@
         <f t="shared" si="0"/>
         <v>bev:maintenance_data</v>
       </c>
-      <c r="B14" t="s">
-        <v>117</v>
-      </c>
       <c r="C14" t="s">
         <v>2</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -1839,14 +1811,11 @@
         <f t="shared" si="0"/>
         <v>bev:production_data</v>
       </c>
-      <c r="B15" t="s">
-        <v>117</v>
-      </c>
       <c r="C15" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -1854,62 +1823,50 @@
         <f t="shared" si="0"/>
         <v>bev:availability_kpis</v>
       </c>
-      <c r="B16" t="s">
-        <v>117</v>
-      </c>
       <c r="C16" t="s">
+        <v>295</v>
+      </c>
+      <c r="F16" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="F16" s="2" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
         <f t="shared" si="0"/>
         <v>bev:utilization_kpis</v>
       </c>
-      <c r="B17" t="s">
-        <v>117</v>
-      </c>
       <c r="C17" t="s">
+        <v>296</v>
+      </c>
+      <c r="F17" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="F17" s="2" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
         <f t="shared" si="0"/>
         <v>bev:effectiveness_kpis</v>
       </c>
-      <c r="B18" t="s">
-        <v>117</v>
-      </c>
       <c r="C18" t="s">
+        <v>297</v>
+      </c>
+      <c r="F18" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="F18" s="2" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
         <f t="shared" si="0"/>
         <v>bev:maintenance_kpis</v>
       </c>
-      <c r="B19" t="s">
-        <v>117</v>
-      </c>
       <c r="C19" t="s">
+        <v>298</v>
+      </c>
+      <c r="F19" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="F19" s="2" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
         <f>CONCATENATE("bev:",LOWER(SUBSTITUTE(C20, " ", "_")))</f>
         <v>bev:vehicle_id</v>
@@ -1917,14 +1874,14 @@
       <c r="C20" t="s">
         <v>1</v>
       </c>
-      <c r="E20" t="s">
-        <v>108</v>
-      </c>
       <c r="F20" s="2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+      <c r="J20" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
         <f t="shared" ref="A21:A69" si="1">CONCATENATE("bev:",LOWER(SUBSTITUTE(C21, " ", "_")))</f>
         <v>bev:battery_id</v>
@@ -1932,14 +1889,14 @@
       <c r="C21" t="s">
         <v>12</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="F21" s="2" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J21" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
         <f t="shared" si="1"/>
         <v>bev:fleet_id</v>
@@ -1947,14 +1904,14 @@
       <c r="C22" t="s">
         <v>27</v>
       </c>
-      <c r="E22" t="s">
-        <v>108</v>
-      </c>
       <c r="F22" s="2" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+      <c r="J22" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
         <f t="shared" si="1"/>
         <v>bev:model_year</v>
@@ -1962,14 +1919,14 @@
       <c r="C23" t="s">
         <v>28</v>
       </c>
-      <c r="E23" t="s">
-        <v>237</v>
-      </c>
       <c r="F23" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J23" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
         <f t="shared" si="1"/>
         <v>bev:initial_service_year</v>
@@ -1977,29 +1934,29 @@
       <c r="C24" t="s">
         <v>29</v>
       </c>
-      <c r="E24" t="s">
-        <v>237</v>
-      </c>
       <c r="F24" s="2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="J24" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
         <f t="shared" si="1"/>
         <v>bev:rebuild_count</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="E25" t="s">
-        <v>108</v>
+        <v>248</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J25" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
         <f t="shared" si="1"/>
         <v>bev:last_rebuild_year</v>
@@ -2007,14 +1964,14 @@
       <c r="C26" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E26" t="s">
-        <v>108</v>
-      </c>
       <c r="F26" s="2" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+      <c r="J26" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
         <f t="shared" si="1"/>
         <v>bev:model_name</v>
@@ -2022,14 +1979,14 @@
       <c r="C27" t="s">
         <v>30</v>
       </c>
-      <c r="E27" t="s">
-        <v>237</v>
-      </c>
       <c r="F27" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+      <c r="J27" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="str">
         <f t="shared" si="1"/>
         <v>bev:manufacturer</v>
@@ -2037,29 +1994,29 @@
       <c r="C28" t="s">
         <v>31</v>
       </c>
-      <c r="E28" t="s">
-        <v>237</v>
-      </c>
       <c r="F28" s="2" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>249</v>
+      </c>
+      <c r="J28" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" t="str">
         <f t="shared" si="1"/>
         <v>bev:functional_location</v>
       </c>
       <c r="C29" t="s">
-        <v>327</v>
-      </c>
-      <c r="E29" t="s">
-        <v>237</v>
+        <v>319</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+        <v>320</v>
+      </c>
+      <c r="J29" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
         <f t="shared" si="1"/>
         <v>bev:energy_system_architecture</v>
@@ -2067,35 +2024,35 @@
       <c r="C30" t="s">
         <v>58</v>
       </c>
-      <c r="E30" t="s">
-        <v>108</v>
-      </c>
       <c r="F30" s="2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>321</v>
+      </c>
+      <c r="J30" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" t="str">
         <f t="shared" si="1"/>
         <v>bev:vehicle_type</v>
       </c>
       <c r="C31" t="s">
-        <v>234</v>
-      </c>
-      <c r="E31" t="s">
-        <v>108</v>
+        <v>231</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>322</v>
+      </c>
+      <c r="J31" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" t="str">
         <f t="shared" si="1"/>
         <v>bev:vehicle_class</v>
@@ -2103,14 +2060,14 @@
       <c r="C32" t="s">
         <v>44</v>
       </c>
-      <c r="E32" t="s">
-        <v>108</v>
-      </c>
       <c r="F32" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>331</v>
+        <v>323</v>
+      </c>
+      <c r="J32" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -2121,14 +2078,14 @@
       <c r="C33" t="s">
         <v>64</v>
       </c>
-      <c r="E33" t="s">
-        <v>108</v>
-      </c>
       <c r="F33" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>332</v>
+        <v>324</v>
+      </c>
+      <c r="J33" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -2139,11 +2096,11 @@
       <c r="C34" t="s">
         <v>32</v>
       </c>
-      <c r="E34" t="s">
-        <v>108</v>
-      </c>
       <c r="F34" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
+      </c>
+      <c r="J34" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -2152,16 +2109,16 @@
         <v>bev:gross_vehicle_weight</v>
       </c>
       <c r="C35" t="s">
-        <v>134</v>
-      </c>
-      <c r="E35" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
+      </c>
+      <c r="J35" t="s">
+        <v>107</v>
       </c>
       <c r="K35" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
@@ -2170,13 +2127,13 @@
         <v>bev:purchase_cost</v>
       </c>
       <c r="C36" t="s">
-        <v>113</v>
-      </c>
-      <c r="E36" t="s">
-        <v>237</v>
+        <v>112</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>254</v>
+        <v>250</v>
+      </c>
+      <c r="J36" t="s">
+        <v>337</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -2187,11 +2144,11 @@
       <c r="C37" t="s">
         <v>33</v>
       </c>
-      <c r="E37" t="s">
-        <v>108</v>
-      </c>
       <c r="F37" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
+      </c>
+      <c r="J37" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -2202,11 +2159,11 @@
       <c r="C38" t="s">
         <v>34</v>
       </c>
-      <c r="E38" t="s">
-        <v>108</v>
-      </c>
       <c r="F38" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
+      </c>
+      <c r="J38" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -2217,11 +2174,11 @@
       <c r="C39" t="s">
         <v>35</v>
       </c>
-      <c r="E39" t="s">
-        <v>108</v>
-      </c>
       <c r="F39" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
+      </c>
+      <c r="J39" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
@@ -2232,11 +2189,11 @@
       <c r="C40" t="s">
         <v>36</v>
       </c>
-      <c r="E40" t="s">
-        <v>108</v>
-      </c>
       <c r="F40" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
+      </c>
+      <c r="J40" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -2245,16 +2202,16 @@
         <v>bev:auxiliary_powered_heater</v>
       </c>
       <c r="C41" t="s">
+        <v>106</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="J41" t="s">
         <v>107</v>
-      </c>
-      <c r="E41" t="s">
-        <v>108</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>333</v>
-      </c>
-      <c r="H41" s="2" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -2265,11 +2222,11 @@
       <c r="C42" t="s">
         <v>39</v>
       </c>
-      <c r="E42" t="s">
-        <v>108</v>
-      </c>
       <c r="F42" s="2" t="s">
-        <v>140</v>
+        <v>137</v>
+      </c>
+      <c r="J42" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="43" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -2278,16 +2235,16 @@
         <v>bev:charge_connector</v>
       </c>
       <c r="C43" t="s">
-        <v>343</v>
-      </c>
-      <c r="E43" t="s">
-        <v>108</v>
+        <v>335</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>335</v>
+        <v>327</v>
+      </c>
+      <c r="J43" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -2296,13 +2253,13 @@
         <v>bev:measurement_start</v>
       </c>
       <c r="C44" t="s">
-        <v>145</v>
-      </c>
-      <c r="E44" t="s">
-        <v>237</v>
+        <v>142</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>142</v>
+        <v>139</v>
+      </c>
+      <c r="J44" t="s">
+        <v>337</v>
       </c>
     </row>
     <row r="45" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -2311,13 +2268,13 @@
         <v>bev:measurement_end</v>
       </c>
       <c r="C45" t="s">
-        <v>146</v>
-      </c>
-      <c r="E45" t="s">
-        <v>237</v>
+        <v>143</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
+      </c>
+      <c r="J45" t="s">
+        <v>337</v>
       </c>
     </row>
     <row r="46" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -2328,11 +2285,11 @@
       <c r="C46" t="s">
         <v>65</v>
       </c>
-      <c r="E46" t="s">
-        <v>108</v>
-      </c>
       <c r="F46" s="2" t="s">
         <v>81</v>
+      </c>
+      <c r="J46" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="47" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -2343,11 +2300,11 @@
       <c r="C47" t="s">
         <v>11</v>
       </c>
-      <c r="E47" t="s">
-        <v>108</v>
-      </c>
       <c r="F47" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
+      </c>
+      <c r="J47" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
@@ -2356,16 +2313,16 @@
         <v>bev:vehicle_idling_time</v>
       </c>
       <c r="C48" t="s">
-        <v>340</v>
-      </c>
-      <c r="E48" t="s">
-        <v>108</v>
+        <v>332</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+      <c r="J48" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="str">
         <f t="shared" si="1"/>
         <v>bev:driving_time</v>
@@ -2373,14 +2330,14 @@
       <c r="C49" t="s">
         <v>4</v>
       </c>
-      <c r="E49" t="s">
-        <v>108</v>
-      </c>
       <c r="F49" s="2" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+      <c r="J49" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="str">
         <f t="shared" si="1"/>
         <v>bev:total_run_time</v>
@@ -2388,14 +2345,14 @@
       <c r="C50" t="s">
         <v>5</v>
       </c>
-      <c r="E50" t="s">
-        <v>108</v>
-      </c>
       <c r="F50" s="2" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+      <c r="J50" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="str">
         <f t="shared" ref="A51:A58" si="2">CONCATENATE("bev:",LOWER(SUBSTITUTE(C51, " ", "_")))</f>
         <v>bev:queue_time</v>
@@ -2403,14 +2360,14 @@
       <c r="C51" t="s">
         <v>72</v>
       </c>
-      <c r="E51" t="s">
-        <v>108</v>
-      </c>
       <c r="F51" s="2" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+      <c r="J51" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="str">
         <f t="shared" si="2"/>
         <v>bev:battery_swapping_time</v>
@@ -2418,14 +2375,14 @@
       <c r="C52" t="s">
         <v>73</v>
       </c>
-      <c r="E52" t="s">
-        <v>108</v>
-      </c>
       <c r="F52" s="2" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+      <c r="J52" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A53" t="str">
         <f t="shared" si="2"/>
         <v>bev:start_location</v>
@@ -2433,14 +2390,14 @@
       <c r="C53" t="s">
         <v>68</v>
       </c>
-      <c r="E53" t="s">
-        <v>108</v>
-      </c>
       <c r="F53" s="2" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+      <c r="J53" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A54" t="str">
         <f t="shared" si="2"/>
         <v>bev:end_location</v>
@@ -2448,14 +2405,14 @@
       <c r="C54" t="s">
         <v>69</v>
       </c>
-      <c r="E54" t="s">
-        <v>108</v>
-      </c>
       <c r="F54" s="2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+      <c r="J54" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" t="str">
         <f t="shared" si="2"/>
         <v>bev:location</v>
@@ -2463,14 +2420,14 @@
       <c r="C55" t="s">
         <v>67</v>
       </c>
-      <c r="E55" t="s">
-        <v>108</v>
-      </c>
       <c r="F55" s="2" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>318</v>
+      </c>
+      <c r="J55" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" t="str">
         <f t="shared" si="2"/>
         <v>bev:average_speed</v>
@@ -2478,14 +2435,14 @@
       <c r="C56" t="s">
         <v>20</v>
       </c>
-      <c r="E56" t="s">
-        <v>108</v>
-      </c>
       <c r="F56" s="2" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+      <c r="J56" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="str">
         <f t="shared" si="2"/>
         <v>bev:speed</v>
@@ -2493,14 +2450,14 @@
       <c r="C57" t="s">
         <v>70</v>
       </c>
-      <c r="E57" t="s">
-        <v>108</v>
-      </c>
       <c r="F57" s="2" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+      <c r="J57" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="str">
         <f t="shared" si="2"/>
         <v>bev:acceleration</v>
@@ -2508,14 +2465,14 @@
       <c r="C58" t="s">
         <v>71</v>
       </c>
-      <c r="E58" t="s">
-        <v>108</v>
-      </c>
       <c r="F58" s="2" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+      <c r="J58" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" t="str">
         <f t="shared" si="1"/>
         <v>bev:number_of_charging_sessions</v>
@@ -2523,14 +2480,14 @@
       <c r="C59" t="s">
         <v>47</v>
       </c>
-      <c r="E59" t="s">
-        <v>108</v>
-      </c>
       <c r="F59" s="2" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+      <c r="J59" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" t="str">
         <f t="shared" si="1"/>
         <v>bev:average_ambient_temperature</v>
@@ -2538,14 +2495,14 @@
       <c r="C60" t="s">
         <v>16</v>
       </c>
-      <c r="E60" t="s">
-        <v>108</v>
-      </c>
       <c r="F60" s="2" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+      <c r="J60" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" t="str">
         <f t="shared" si="1"/>
         <v>bev:initial_odometer</v>
@@ -2553,14 +2510,14 @@
       <c r="C61" t="s">
         <v>9</v>
       </c>
-      <c r="E61" t="s">
-        <v>108</v>
-      </c>
       <c r="F61" s="2" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+      <c r="J61" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" t="str">
         <f t="shared" si="1"/>
         <v>bev:final_odometer</v>
@@ -2568,14 +2525,14 @@
       <c r="C62" t="s">
         <v>10</v>
       </c>
-      <c r="E62" t="s">
-        <v>108</v>
-      </c>
       <c r="F62" s="2" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+      <c r="J62" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="str">
         <f>CONCATENATE("bev:",LOWER(SUBSTITUTE(C63, " ", "_")))</f>
         <v>bev:traction_energy</v>
@@ -2583,14 +2540,14 @@
       <c r="C63" t="s">
         <v>19</v>
       </c>
-      <c r="E63" t="s">
-        <v>108</v>
-      </c>
       <c r="F63" s="2" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+      <c r="J63" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="str">
         <f>CONCATENATE("bev:",LOWER(SUBSTITUTE(C64, " ", "_")))</f>
         <v>bev:hydraulic_system_energy</v>
@@ -2598,14 +2555,14 @@
       <c r="C64" t="s">
         <v>83</v>
       </c>
-      <c r="E64" t="s">
-        <v>108</v>
-      </c>
       <c r="F64" s="2" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+      <c r="J64" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" t="str">
         <f>CONCATENATE("bev:",LOWER(SUBSTITUTE(C65, " ", "_")))</f>
         <v>bev:hydraulic_system_power</v>
@@ -2613,14 +2570,14 @@
       <c r="C65" t="s">
         <v>82</v>
       </c>
-      <c r="E65" t="s">
-        <v>108</v>
-      </c>
       <c r="F65" s="2" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+      <c r="J65" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A66" t="str">
         <f t="shared" si="1"/>
         <v>bev:hv_accessories_energy</v>
@@ -2628,14 +2585,14 @@
       <c r="C66" t="s">
         <v>17</v>
       </c>
-      <c r="E66" t="s">
-        <v>108</v>
-      </c>
       <c r="F66" s="2" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+      <c r="J66" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" t="str">
         <f t="shared" si="1"/>
         <v>bev:lv_accessories_energy</v>
@@ -2643,14 +2600,14 @@
       <c r="C67" t="s">
         <v>18</v>
       </c>
-      <c r="E67" t="s">
-        <v>108</v>
-      </c>
       <c r="F67" s="2" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+        <v>162</v>
+      </c>
+      <c r="J67" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" t="str">
         <f t="shared" si="1"/>
         <v>bev:payload</v>
@@ -2658,29 +2615,29 @@
       <c r="C68" t="s">
         <v>90</v>
       </c>
-      <c r="E68" t="s">
-        <v>108</v>
-      </c>
       <c r="F68" s="2" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+      <c r="J68" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A69" t="str">
         <f t="shared" si="1"/>
         <v>bev:inclination</v>
       </c>
       <c r="C69" t="s">
-        <v>156</v>
-      </c>
-      <c r="E69" t="s">
-        <v>108</v>
+        <v>153</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+      <c r="J69" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" t="str">
         <f t="shared" ref="A70:A136" si="3">CONCATENATE("bev:",LOWER(SUBSTITUTE(C70, " ", "_")))</f>
         <v>bev:alert_id</v>
@@ -2688,14 +2645,14 @@
       <c r="C70" t="s">
         <v>77</v>
       </c>
-      <c r="E70" t="s">
-        <v>237</v>
-      </c>
       <c r="F70" s="2" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+      <c r="J70" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" t="str">
         <f t="shared" si="3"/>
         <v>bev:alert_type</v>
@@ -2703,14 +2660,14 @@
       <c r="C71" t="s">
         <v>78</v>
       </c>
-      <c r="E71" t="s">
-        <v>237</v>
-      </c>
       <c r="F71" s="2" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+        <v>167</v>
+      </c>
+      <c r="J71" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" t="str">
         <f t="shared" si="3"/>
         <v>bev:alert_description</v>
@@ -2718,29 +2675,29 @@
       <c r="C72" t="s">
         <v>79</v>
       </c>
-      <c r="E72" t="s">
-        <v>237</v>
-      </c>
       <c r="F72" s="2" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+      <c r="J72" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" t="str">
         <f t="shared" si="3"/>
         <v>bev:alert_date_time</v>
       </c>
       <c r="C73" t="s">
-        <v>336</v>
-      </c>
-      <c r="E73" t="s">
-        <v>237</v>
+        <v>328</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+      <c r="J73" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" t="str">
         <f t="shared" si="3"/>
         <v>bev:alert_status</v>
@@ -2748,14 +2705,14 @@
       <c r="C74" t="s">
         <v>80</v>
       </c>
-      <c r="E74" t="s">
-        <v>237</v>
-      </c>
       <c r="F74" s="2" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+      <c r="J74" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" t="str">
         <f t="shared" si="3"/>
         <v>bev:battery_id</v>
@@ -2763,29 +2720,29 @@
       <c r="C75" t="s">
         <v>12</v>
       </c>
-      <c r="E75" t="s">
-        <v>202</v>
-      </c>
       <c r="F75" s="2" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+      <c r="J75" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A76" t="str">
         <f t="shared" si="3"/>
         <v>bev:pack_id</v>
       </c>
       <c r="C76" t="s">
-        <v>204</v>
-      </c>
-      <c r="E76" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+      <c r="J76" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" t="str">
         <f t="shared" si="3"/>
         <v>bev:module_id</v>
@@ -2793,29 +2750,29 @@
       <c r="C77" t="s">
         <v>23</v>
       </c>
-      <c r="E77" t="s">
+      <c r="F77" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="J77" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" t="str">
+        <f t="shared" si="3"/>
+        <v>bev:cell_id</v>
+      </c>
+      <c r="C78" t="s">
         <v>202</v>
       </c>
-      <c r="F77" s="2" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A78" t="str">
-        <f t="shared" si="3"/>
-        <v>bev:cell_id</v>
-      </c>
-      <c r="C78" t="s">
-        <v>205</v>
-      </c>
-      <c r="E78" t="s">
-        <v>202</v>
-      </c>
       <c r="F78" s="2" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+      <c r="J78" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" t="str">
         <f t="shared" si="3"/>
         <v>bev:battery_chemistry</v>
@@ -2823,17 +2780,17 @@
       <c r="C79" t="s">
         <v>37</v>
       </c>
-      <c r="E79" t="s">
-        <v>202</v>
-      </c>
       <c r="F79" s="2" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="H79" s="2" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+        <v>329</v>
+      </c>
+      <c r="J79" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" t="str">
         <f t="shared" si="3"/>
         <v>bev:manufacturer</v>
@@ -2841,11 +2798,11 @@
       <c r="C80" t="s">
         <v>31</v>
       </c>
-      <c r="E80" t="s">
-        <v>202</v>
-      </c>
       <c r="F80" s="2" t="s">
-        <v>209</v>
+        <v>206</v>
+      </c>
+      <c r="J80" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
@@ -2856,11 +2813,11 @@
       <c r="C81" t="s">
         <v>53</v>
       </c>
-      <c r="E81" t="s">
-        <v>202</v>
-      </c>
       <c r="F81" s="2" t="s">
-        <v>210</v>
+        <v>207</v>
+      </c>
+      <c r="J81" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
@@ -2871,11 +2828,11 @@
       <c r="C82" t="s">
         <v>57</v>
       </c>
-      <c r="E82" t="s">
-        <v>202</v>
-      </c>
       <c r="F82" s="2" t="s">
-        <v>211</v>
+        <v>208</v>
+      </c>
+      <c r="J82" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="83" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -2884,13 +2841,13 @@
         <v>bev:number_of_packs</v>
       </c>
       <c r="C83" t="s">
-        <v>212</v>
-      </c>
-      <c r="E83" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
+      </c>
+      <c r="J83" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
@@ -2901,11 +2858,11 @@
       <c r="C84" t="s">
         <v>38</v>
       </c>
-      <c r="E84" t="s">
-        <v>202</v>
-      </c>
       <c r="F84" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
+      </c>
+      <c r="J84" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
@@ -2916,11 +2873,11 @@
       <c r="C85" t="s">
         <v>54</v>
       </c>
-      <c r="E85" t="s">
-        <v>202</v>
-      </c>
       <c r="F85" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
+      </c>
+      <c r="J85" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.25">
@@ -2929,13 +2886,13 @@
         <v>bev:battery_mass</v>
       </c>
       <c r="C86" t="s">
-        <v>250</v>
-      </c>
-      <c r="E86" t="s">
-        <v>202</v>
+        <v>246</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>251</v>
+        <v>247</v>
+      </c>
+      <c r="J86" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="87" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -2946,11 +2903,11 @@
       <c r="C87" t="s">
         <v>6</v>
       </c>
-      <c r="E87" t="s">
-        <v>202</v>
-      </c>
       <c r="F87" s="2" t="s">
-        <v>216</v>
+        <v>213</v>
+      </c>
+      <c r="J87" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="88" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -2961,11 +2918,11 @@
       <c r="C88" t="s">
         <v>7</v>
       </c>
-      <c r="E88" t="s">
-        <v>202</v>
-      </c>
       <c r="F88" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
+      </c>
+      <c r="J88" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="89" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -2974,16 +2931,16 @@
         <v>bev:soc</v>
       </c>
       <c r="C89" t="s">
-        <v>221</v>
-      </c>
-      <c r="E89" t="s">
-        <v>202</v>
+        <v>218</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>228</v>
+        <v>225</v>
+      </c>
+      <c r="J89" t="s">
+        <v>199</v>
       </c>
       <c r="K89" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="90" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -2994,11 +2951,11 @@
       <c r="C90" t="s">
         <v>8</v>
       </c>
-      <c r="E90" t="s">
-        <v>202</v>
-      </c>
       <c r="F90" s="2" t="s">
-        <v>218</v>
+        <v>215</v>
+      </c>
+      <c r="J90" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="91" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -3007,13 +2964,13 @@
         <v>bev:energy_consumption</v>
       </c>
       <c r="C91" t="s">
+        <v>216</v>
+      </c>
+      <c r="F91" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="E91" t="s">
-        <v>202</v>
-      </c>
-      <c r="F91" s="2" t="s">
-        <v>222</v>
+      <c r="J91" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="92" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -3024,11 +2981,11 @@
       <c r="C92" t="s">
         <v>55</v>
       </c>
-      <c r="E92" t="s">
-        <v>202</v>
-      </c>
       <c r="F92" s="2" t="s">
-        <v>223</v>
+        <v>220</v>
+      </c>
+      <c r="J92" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="93" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -3037,13 +2994,13 @@
         <v>bev:net_energy_consumption</v>
       </c>
       <c r="C93" t="s">
-        <v>220</v>
-      </c>
-      <c r="E93" t="s">
-        <v>202</v>
+        <v>217</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>224</v>
+        <v>221</v>
+      </c>
+      <c r="J93" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="94" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -3054,11 +3011,11 @@
       <c r="C94" t="s">
         <v>21</v>
       </c>
-      <c r="E94" t="s">
-        <v>202</v>
-      </c>
       <c r="F94" s="2" t="s">
-        <v>225</v>
+        <v>222</v>
+      </c>
+      <c r="J94" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="95" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -3069,11 +3026,11 @@
       <c r="C95" t="s">
         <v>22</v>
       </c>
-      <c r="E95" t="s">
-        <v>202</v>
-      </c>
       <c r="F95" s="2" t="s">
-        <v>226</v>
+        <v>223</v>
+      </c>
+      <c r="J95" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.25">
@@ -3084,11 +3041,11 @@
       <c r="C96" t="s">
         <v>24</v>
       </c>
-      <c r="E96" t="s">
-        <v>202</v>
-      </c>
       <c r="F96" s="2" t="s">
-        <v>227</v>
+        <v>224</v>
+      </c>
+      <c r="J96" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.25">
@@ -3099,11 +3056,11 @@
       <c r="C97" t="s">
         <v>25</v>
       </c>
-      <c r="E97" t="s">
-        <v>202</v>
-      </c>
       <c r="F97" s="2" t="s">
-        <v>229</v>
+        <v>226</v>
+      </c>
+      <c r="J97" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.25">
@@ -3114,11 +3071,11 @@
       <c r="C98" t="s">
         <v>26</v>
       </c>
-      <c r="E98" t="s">
-        <v>202</v>
-      </c>
       <c r="F98" s="2" t="s">
-        <v>230</v>
+        <v>227</v>
+      </c>
+      <c r="J98" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.25">
@@ -3129,11 +3086,11 @@
       <c r="C99" t="s">
         <v>76</v>
       </c>
-      <c r="E99" t="s">
-        <v>202</v>
-      </c>
       <c r="F99" s="2" t="s">
-        <v>231</v>
+        <v>228</v>
+      </c>
+      <c r="J99" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="100" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -3144,11 +3101,11 @@
       <c r="C100" t="s">
         <v>75</v>
       </c>
-      <c r="E100" t="s">
-        <v>202</v>
-      </c>
       <c r="F100" s="2" t="s">
-        <v>232</v>
+        <v>229</v>
+      </c>
+      <c r="J100" t="s">
+        <v>199</v>
       </c>
       <c r="K100" t="s">
         <v>75</v>
@@ -3162,11 +3119,11 @@
       <c r="C101" t="s">
         <v>46</v>
       </c>
-      <c r="E101" t="s">
-        <v>233</v>
-      </c>
       <c r="F101" s="2" t="s">
-        <v>235</v>
+        <v>232</v>
+      </c>
+      <c r="J101" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.25">
@@ -3177,11 +3134,11 @@
       <c r="C102" t="s">
         <v>56</v>
       </c>
-      <c r="E102" t="s">
+      <c r="F102" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="F102" s="2" t="s">
-        <v>236</v>
+      <c r="J102" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="103" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -3192,11 +3149,11 @@
       <c r="C103" t="s">
         <v>49</v>
       </c>
-      <c r="E103" t="s">
-        <v>233</v>
-      </c>
       <c r="F103" s="2" t="s">
-        <v>242</v>
+        <v>238</v>
+      </c>
+      <c r="J103" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.25">
@@ -3205,13 +3162,13 @@
         <v>bev:rated_power</v>
       </c>
       <c r="C104" t="s">
-        <v>243</v>
-      </c>
-      <c r="E104" t="s">
-        <v>233</v>
+        <v>239</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>244</v>
+        <v>240</v>
+      </c>
+      <c r="J104" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="105" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -3220,13 +3177,13 @@
         <v>bev:charger_location</v>
       </c>
       <c r="C105" t="s">
-        <v>247</v>
-      </c>
-      <c r="E105" t="s">
-        <v>233</v>
+        <v>243</v>
       </c>
       <c r="F105" s="2" t="s">
-        <v>248</v>
+        <v>244</v>
+      </c>
+      <c r="J105" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="106" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -3237,11 +3194,11 @@
       <c r="C106" t="s">
         <v>51</v>
       </c>
-      <c r="E106" t="s">
-        <v>233</v>
-      </c>
       <c r="F106" s="2" t="s">
-        <v>238</v>
+        <v>234</v>
+      </c>
+      <c r="J106" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="107" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -3252,11 +3209,11 @@
       <c r="C107" t="s">
         <v>52</v>
       </c>
-      <c r="E107" t="s">
-        <v>233</v>
-      </c>
       <c r="F107" s="2" t="s">
-        <v>246</v>
+        <v>242</v>
+      </c>
+      <c r="J107" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.25">
@@ -3267,11 +3224,11 @@
       <c r="C108" t="s">
         <v>48</v>
       </c>
-      <c r="E108" t="s">
-        <v>233</v>
-      </c>
       <c r="F108" s="2" t="s">
-        <v>239</v>
+        <v>235</v>
+      </c>
+      <c r="J108" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="109" spans="1:11" x14ac:dyDescent="0.25">
@@ -3280,13 +3237,13 @@
         <v>bev:charging_power</v>
       </c>
       <c r="C109" t="s">
-        <v>240</v>
-      </c>
-      <c r="E109" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>241</v>
+        <v>237</v>
+      </c>
+      <c r="J109" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="110" spans="1:11" x14ac:dyDescent="0.25">
@@ -3295,19 +3252,19 @@
         <v>bev:charging_rate</v>
       </c>
       <c r="C110" t="s">
-        <v>324</v>
-      </c>
-      <c r="E110" t="s">
-        <v>233</v>
+        <v>316</v>
       </c>
       <c r="F110" s="2" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
       <c r="H110" s="2" t="s">
-        <v>338</v>
+        <v>330</v>
+      </c>
+      <c r="J110" t="s">
+        <v>230</v>
       </c>
       <c r="K110" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
     </row>
     <row r="111" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -3318,11 +3275,11 @@
       <c r="C111" t="s">
         <v>50</v>
       </c>
-      <c r="E111" t="s">
-        <v>233</v>
-      </c>
       <c r="F111" s="2" t="s">
-        <v>245</v>
+        <v>241</v>
+      </c>
+      <c r="J111" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="112" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -3331,13 +3288,13 @@
         <v>bev:work_order_id</v>
       </c>
       <c r="C112" t="s">
-        <v>118</v>
-      </c>
-      <c r="E112" t="s">
-        <v>249</v>
+        <v>116</v>
       </c>
       <c r="F112" s="2" t="s">
-        <v>255</v>
+        <v>251</v>
+      </c>
+      <c r="J112" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="113" spans="1:11" x14ac:dyDescent="0.25">
@@ -3346,13 +3303,13 @@
         <v>bev:work_order_description</v>
       </c>
       <c r="C113" t="s">
-        <v>256</v>
-      </c>
-      <c r="E113" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="F113" s="2" t="s">
-        <v>257</v>
+        <v>253</v>
+      </c>
+      <c r="J113" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="114" spans="1:11" x14ac:dyDescent="0.25">
@@ -3361,13 +3318,13 @@
         <v>bev:work_order_status</v>
       </c>
       <c r="C114" t="s">
-        <v>258</v>
-      </c>
-      <c r="E114" t="s">
-        <v>249</v>
+        <v>254</v>
       </c>
       <c r="F114" s="2" t="s">
-        <v>259</v>
+        <v>255</v>
+      </c>
+      <c r="J114" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="115" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -3378,11 +3335,11 @@
       <c r="C115" t="s">
         <v>59</v>
       </c>
-      <c r="E115" t="s">
-        <v>249</v>
-      </c>
       <c r="F115" s="2" t="s">
-        <v>260</v>
+        <v>256</v>
+      </c>
+      <c r="J115" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="116" spans="1:11" x14ac:dyDescent="0.25">
@@ -3393,11 +3350,11 @@
       <c r="C116" t="s">
         <v>61</v>
       </c>
-      <c r="E116" t="s">
-        <v>249</v>
-      </c>
       <c r="F116" s="2" t="s">
-        <v>261</v>
+        <v>257</v>
+      </c>
+      <c r="J116" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="117" spans="1:11" x14ac:dyDescent="0.25">
@@ -3408,11 +3365,11 @@
       <c r="C117" t="s">
         <v>62</v>
       </c>
-      <c r="E117" t="s">
-        <v>249</v>
-      </c>
       <c r="F117" s="2" t="s">
-        <v>262</v>
+        <v>258</v>
+      </c>
+      <c r="J117" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="118" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -3423,11 +3380,11 @@
       <c r="C118" t="s">
         <v>60</v>
       </c>
-      <c r="E118" t="s">
-        <v>249</v>
-      </c>
       <c r="F118" s="2" t="s">
-        <v>263</v>
+        <v>259</v>
+      </c>
+      <c r="J118" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="119" spans="1:11" x14ac:dyDescent="0.25">
@@ -3436,13 +3393,13 @@
         <v>bev:work_order_start</v>
       </c>
       <c r="C119" t="s">
-        <v>264</v>
-      </c>
-      <c r="E119" t="s">
-        <v>249</v>
+        <v>260</v>
       </c>
       <c r="F119" s="2" t="s">
-        <v>266</v>
+        <v>262</v>
+      </c>
+      <c r="J119" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="120" spans="1:11" x14ac:dyDescent="0.25">
@@ -3451,13 +3408,13 @@
         <v>bev:work_order_end</v>
       </c>
       <c r="C120" t="s">
-        <v>265</v>
-      </c>
-      <c r="E120" t="s">
-        <v>249</v>
+        <v>261</v>
       </c>
       <c r="F120" s="2" t="s">
-        <v>267</v>
+        <v>263</v>
+      </c>
+      <c r="J120" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="121" spans="1:11" x14ac:dyDescent="0.25">
@@ -3468,11 +3425,11 @@
       <c r="C121" t="s">
         <v>63</v>
       </c>
-      <c r="E121" t="s">
-        <v>249</v>
-      </c>
       <c r="F121" s="2" t="s">
-        <v>268</v>
+        <v>264</v>
+      </c>
+      <c r="J121" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="122" spans="1:11" x14ac:dyDescent="0.25">
@@ -3481,13 +3438,13 @@
         <v>bev:part_costs</v>
       </c>
       <c r="C122" t="s">
-        <v>119</v>
-      </c>
-      <c r="E122" t="s">
-        <v>249</v>
+        <v>117</v>
       </c>
       <c r="F122" s="2" t="s">
-        <v>269</v>
+        <v>265</v>
+      </c>
+      <c r="J122" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="123" spans="1:11" x14ac:dyDescent="0.25">
@@ -3496,13 +3453,13 @@
         <v>bev:labour_costs</v>
       </c>
       <c r="C123" t="s">
-        <v>120</v>
-      </c>
-      <c r="E123" t="s">
-        <v>249</v>
+        <v>118</v>
       </c>
       <c r="F123" s="2" t="s">
-        <v>270</v>
+        <v>266</v>
+      </c>
+      <c r="J123" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="124" spans="1:11" x14ac:dyDescent="0.25">
@@ -3511,13 +3468,13 @@
         <v>bev:time_in_workshop</v>
       </c>
       <c r="C124" t="s">
-        <v>196</v>
-      </c>
-      <c r="E124" t="s">
-        <v>249</v>
+        <v>193</v>
       </c>
       <c r="F124" s="2" t="s">
-        <v>271</v>
+        <v>267</v>
+      </c>
+      <c r="J124" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="125" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -3526,13 +3483,13 @@
         <v>bev:logistic_delay</v>
       </c>
       <c r="C125" t="s">
-        <v>197</v>
-      </c>
-      <c r="E125" t="s">
-        <v>249</v>
+        <v>194</v>
       </c>
       <c r="F125" s="2" t="s">
-        <v>272</v>
+        <v>268</v>
+      </c>
+      <c r="J125" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="126" spans="1:11" x14ac:dyDescent="0.25">
@@ -3541,16 +3498,16 @@
         <v>bev:time_to_repair</v>
       </c>
       <c r="C126" t="s">
-        <v>198</v>
-      </c>
-      <c r="E126" t="s">
-        <v>249</v>
+        <v>195</v>
       </c>
       <c r="F126" s="2" t="s">
-        <v>273</v>
+        <v>269</v>
+      </c>
+      <c r="J126" t="s">
+        <v>245</v>
       </c>
       <c r="K126" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
     </row>
     <row r="127" spans="1:11" x14ac:dyDescent="0.25">
@@ -3559,13 +3516,13 @@
         <v>bev:idle_time</v>
       </c>
       <c r="C127" t="s">
-        <v>199</v>
-      </c>
-      <c r="E127" t="s">
-        <v>249</v>
+        <v>196</v>
       </c>
       <c r="F127" s="2" t="s">
-        <v>275</v>
+        <v>271</v>
+      </c>
+      <c r="J127" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="128" spans="1:11" x14ac:dyDescent="0.25">
@@ -3576,11 +3533,11 @@
       <c r="C128" t="s">
         <v>87</v>
       </c>
-      <c r="E128" t="s">
-        <v>310</v>
-      </c>
       <c r="F128" s="2" t="s">
-        <v>276</v>
+        <v>272</v>
+      </c>
+      <c r="J128" t="s">
+        <v>338</v>
       </c>
       <c r="K128" t="s">
         <v>13</v>
@@ -3592,13 +3549,13 @@
         <v>bev:mean_time_between_failures</v>
       </c>
       <c r="C129" t="s">
-        <v>200</v>
-      </c>
-      <c r="E129" t="s">
-        <v>310</v>
+        <v>197</v>
       </c>
       <c r="F129" s="2" t="s">
-        <v>277</v>
+        <v>273</v>
+      </c>
+      <c r="J129" t="s">
+        <v>338</v>
       </c>
       <c r="K129" t="s">
         <v>14</v>
@@ -3612,11 +3569,11 @@
       <c r="C130" t="s">
         <v>66</v>
       </c>
-      <c r="E130" t="s">
-        <v>310</v>
-      </c>
       <c r="F130" s="2" t="s">
-        <v>278</v>
+        <v>274</v>
+      </c>
+      <c r="J130" t="s">
+        <v>338</v>
       </c>
       <c r="K130" t="s">
         <v>15</v>
@@ -3628,13 +3585,13 @@
         <v>bev:mean_down_time</v>
       </c>
       <c r="C131" t="s">
-        <v>201</v>
-      </c>
-      <c r="E131" t="s">
-        <v>310</v>
+        <v>198</v>
       </c>
       <c r="F131" s="2" t="s">
-        <v>274</v>
+        <v>270</v>
+      </c>
+      <c r="J131" t="s">
+        <v>338</v>
       </c>
       <c r="K131" t="s">
         <v>84</v>
@@ -3646,13 +3603,13 @@
         <v>bev:calendar_time</v>
       </c>
       <c r="C132" t="s">
-        <v>176</v>
-      </c>
-      <c r="E132" t="s">
-        <v>279</v>
+        <v>173</v>
       </c>
       <c r="F132" s="2" t="s">
-        <v>282</v>
+        <v>278</v>
+      </c>
+      <c r="J132" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="133" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -3661,13 +3618,13 @@
         <v>bev:scheduled_time</v>
       </c>
       <c r="C133" t="s">
-        <v>177</v>
-      </c>
-      <c r="E133" t="s">
-        <v>279</v>
+        <v>174</v>
       </c>
       <c r="F133" s="2" t="s">
-        <v>286</v>
+        <v>282</v>
+      </c>
+      <c r="J133" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="134" spans="1:11" x14ac:dyDescent="0.25">
@@ -3676,13 +3633,13 @@
         <v>bev:unscheduled_time</v>
       </c>
       <c r="C134" t="s">
-        <v>192</v>
-      </c>
-      <c r="E134" t="s">
+        <v>189</v>
+      </c>
+      <c r="F134" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="F134" s="2" t="s">
-        <v>283</v>
+      <c r="J134" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="135" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -3691,16 +3648,16 @@
         <v>bev:down_time</v>
       </c>
       <c r="C135" t="s">
+        <v>276</v>
+      </c>
+      <c r="F135" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="E135" t="s">
-        <v>279</v>
-      </c>
-      <c r="F135" s="2" t="s">
-        <v>284</v>
+      <c r="J135" t="s">
+        <v>275</v>
       </c>
       <c r="K135" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
     </row>
     <row r="136" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -3709,13 +3666,13 @@
         <v>bev:available_time</v>
       </c>
       <c r="C136" t="s">
-        <v>178</v>
-      </c>
-      <c r="E136" t="s">
-        <v>279</v>
+        <v>175</v>
       </c>
       <c r="F136" s="2" t="s">
-        <v>285</v>
+        <v>281</v>
+      </c>
+      <c r="J136" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="137" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -3724,13 +3681,13 @@
         <v>bev:standby_time</v>
       </c>
       <c r="C137" t="s">
-        <v>193</v>
-      </c>
-      <c r="E137" t="s">
-        <v>279</v>
+        <v>190</v>
       </c>
       <c r="F137" s="2" t="s">
-        <v>290</v>
+        <v>286</v>
+      </c>
+      <c r="J137" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="138" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -3739,13 +3696,13 @@
         <v>bev:operating_standby_time</v>
       </c>
       <c r="C138" t="s">
-        <v>182</v>
-      </c>
-      <c r="E138" t="s">
-        <v>279</v>
+        <v>179</v>
       </c>
       <c r="F138" s="2" t="s">
-        <v>288</v>
+        <v>284</v>
+      </c>
+      <c r="J138" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="139" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -3754,13 +3711,13 @@
         <v>bev:external_standby_time</v>
       </c>
       <c r="C139" t="s">
-        <v>183</v>
-      </c>
-      <c r="E139" t="s">
-        <v>279</v>
+        <v>180</v>
       </c>
       <c r="F139" s="2" t="s">
-        <v>287</v>
+        <v>283</v>
+      </c>
+      <c r="J139" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="140" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -3769,13 +3726,13 @@
         <v>bev:operating_time</v>
       </c>
       <c r="C140" t="s">
-        <v>179</v>
-      </c>
-      <c r="E140" t="s">
-        <v>279</v>
+        <v>176</v>
       </c>
       <c r="F140" s="2" t="s">
-        <v>289</v>
+        <v>285</v>
+      </c>
+      <c r="J140" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="141" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -3784,13 +3741,13 @@
         <v>bev:operating_delay</v>
       </c>
       <c r="C141" t="s">
-        <v>194</v>
-      </c>
-      <c r="E141" t="s">
-        <v>279</v>
+        <v>191</v>
       </c>
       <c r="F141" s="2" t="s">
-        <v>291</v>
+        <v>287</v>
+      </c>
+      <c r="J141" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="142" spans="1:11" ht="75" x14ac:dyDescent="0.25">
@@ -3799,13 +3756,13 @@
         <v>bev:working_time</v>
       </c>
       <c r="C142" t="s">
-        <v>180</v>
-      </c>
-      <c r="E142" t="s">
-        <v>279</v>
+        <v>177</v>
       </c>
       <c r="F142" s="2" t="s">
-        <v>292</v>
+        <v>288</v>
+      </c>
+      <c r="J142" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="143" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -3814,13 +3771,13 @@
         <v>bev:non-productive_time</v>
       </c>
       <c r="C143" t="s">
-        <v>195</v>
-      </c>
-      <c r="E143" t="s">
-        <v>279</v>
+        <v>192</v>
       </c>
       <c r="F143" s="2" t="s">
-        <v>293</v>
+        <v>289</v>
+      </c>
+      <c r="J143" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="144" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -3829,13 +3786,13 @@
         <v>bev:productive_time</v>
       </c>
       <c r="C144" t="s">
-        <v>181</v>
-      </c>
-      <c r="E144" t="s">
-        <v>279</v>
+        <v>178</v>
       </c>
       <c r="F144" s="2" t="s">
-        <v>294</v>
+        <v>290</v>
+      </c>
+      <c r="J144" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="145" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -3844,16 +3801,16 @@
         <v>bev:up_time</v>
       </c>
       <c r="C145" t="s">
-        <v>281</v>
-      </c>
-      <c r="E145" t="s">
-        <v>307</v>
+        <v>277</v>
       </c>
       <c r="F145" s="2" t="s">
-        <v>295</v>
+        <v>291</v>
+      </c>
+      <c r="J145" t="s">
+        <v>339</v>
       </c>
       <c r="K145" t="s">
-        <v>323</v>
+        <v>315</v>
       </c>
     </row>
     <row r="146" spans="1:11" ht="75" x14ac:dyDescent="0.25">
@@ -3862,13 +3819,13 @@
         <v>bev:availability</v>
       </c>
       <c r="C146" t="s">
-        <v>296</v>
-      </c>
-      <c r="E146" t="s">
-        <v>307</v>
+        <v>292</v>
       </c>
       <c r="F146" s="2" t="s">
-        <v>319</v>
+        <v>311</v>
+      </c>
+      <c r="J146" t="s">
+        <v>339</v>
       </c>
     </row>
     <row r="147" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -3877,13 +3834,13 @@
         <v>bev:physical_availability</v>
       </c>
       <c r="C147" t="s">
-        <v>184</v>
-      </c>
-      <c r="E147" t="s">
-        <v>307</v>
+        <v>181</v>
       </c>
       <c r="F147" s="2" t="s">
-        <v>297</v>
+        <v>293</v>
+      </c>
+      <c r="J147" t="s">
+        <v>339</v>
       </c>
     </row>
     <row r="148" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -3892,13 +3849,13 @@
         <v>bev:mechanical_availability</v>
       </c>
       <c r="C148" t="s">
-        <v>185</v>
-      </c>
-      <c r="E148" t="s">
-        <v>307</v>
+        <v>182</v>
       </c>
       <c r="F148" s="2" t="s">
-        <v>298</v>
+        <v>294</v>
+      </c>
+      <c r="J148" t="s">
+        <v>339</v>
       </c>
     </row>
     <row r="149" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -3907,13 +3864,13 @@
         <v>bev:use_of_availability</v>
       </c>
       <c r="C149" t="s">
-        <v>186</v>
-      </c>
-      <c r="E149" t="s">
-        <v>308</v>
+        <v>183</v>
       </c>
       <c r="F149" s="2" t="s">
-        <v>311</v>
+        <v>303</v>
+      </c>
+      <c r="J149" t="s">
+        <v>340</v>
       </c>
     </row>
     <row r="150" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -3922,13 +3879,13 @@
         <v>bev:asset_utilization</v>
       </c>
       <c r="C150" t="s">
-        <v>187</v>
-      </c>
-      <c r="E150" t="s">
-        <v>308</v>
+        <v>184</v>
       </c>
       <c r="F150" s="2" t="s">
-        <v>312</v>
+        <v>304</v>
+      </c>
+      <c r="J150" t="s">
+        <v>340</v>
       </c>
     </row>
     <row r="151" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -3937,13 +3894,13 @@
         <v>bev:operating_utilization</v>
       </c>
       <c r="C151" t="s">
-        <v>188</v>
-      </c>
-      <c r="E151" t="s">
-        <v>308</v>
+        <v>185</v>
       </c>
       <c r="F151" s="2" t="s">
-        <v>313</v>
+        <v>305</v>
+      </c>
+      <c r="J151" t="s">
+        <v>340</v>
       </c>
     </row>
     <row r="152" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -3952,13 +3909,13 @@
         <v>bev:effective_utilization</v>
       </c>
       <c r="C152" t="s">
-        <v>189</v>
-      </c>
-      <c r="E152" t="s">
-        <v>308</v>
+        <v>186</v>
       </c>
       <c r="F152" s="2" t="s">
-        <v>314</v>
+        <v>306</v>
+      </c>
+      <c r="J152" t="s">
+        <v>340</v>
       </c>
     </row>
     <row r="153" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -3967,13 +3924,13 @@
         <v>bev:operating_efficiency</v>
       </c>
       <c r="C153" t="s">
-        <v>190</v>
-      </c>
-      <c r="E153" t="s">
-        <v>309</v>
+        <v>187</v>
       </c>
       <c r="F153" s="2" t="s">
-        <v>315</v>
+        <v>307</v>
+      </c>
+      <c r="J153" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="154" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -3982,13 +3939,13 @@
         <v>bev:production_effectiveness</v>
       </c>
       <c r="C154" t="s">
-        <v>191</v>
-      </c>
-      <c r="E154" t="s">
-        <v>309</v>
+        <v>188</v>
       </c>
       <c r="F154" s="2" t="s">
-        <v>316</v>
+        <v>308</v>
+      </c>
+      <c r="J154" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="155" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -3999,11 +3956,11 @@
       <c r="C155" t="s">
         <v>89</v>
       </c>
-      <c r="E155" t="s">
-        <v>309</v>
-      </c>
       <c r="F155" s="2" t="s">
-        <v>318</v>
+        <v>310</v>
+      </c>
+      <c r="J155" t="s">
+        <v>341</v>
       </c>
       <c r="K155" t="s">
         <v>88</v>
@@ -4017,11 +3974,11 @@
       <c r="C156" t="s">
         <v>86</v>
       </c>
-      <c r="E156" t="s">
-        <v>279</v>
-      </c>
       <c r="F156" s="2" t="s">
-        <v>317</v>
+        <v>309</v>
+      </c>
+      <c r="J156" t="s">
+        <v>275</v>
       </c>
       <c r="K156" t="s">
         <v>85</v>
@@ -4034,6 +3991,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009ECF0953322C9541A9A1EDFD15376FEB" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="be6ec5c2eb01e6dab00300863d7ca40e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d1e4d1e0-c95d-4c51-be4d-468b7a581b67" xmlns:ns3="d8e165db-149b-4197-bc76-0f068cbb73e1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cba18d3b1191ba2ed2ca6b2456b1847e" ns2:_="" ns3:_="">
     <xsd:import namespace="d1e4d1e0-c95d-4c51-be4d-468b7a581b67"/>
@@ -4244,15 +4210,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -4264,6 +4221,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B902C61F-C425-480E-9AE8-5743FFC97C42}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4BFD419B-CB92-44D3-B027-0EE3D3BB0D32}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4282,14 +4247,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B902C61F-C425-480E-9AE8-5743FFC97C42}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0058CAD2-89AE-44C8-AF19-A0D04C3633AC}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Removing redundant "model" entity
</commit_message>
<xml_diff>
--- a/BEV Data Vocabulary.xlsx
+++ b/BEV Data Vocabulary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edwar\Github\evmo-vocab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5280F41E-ECE8-476B-86AD-AADC2D3D9DCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CC1F5B6-F0F0-49EE-B0AF-ADE7BF219E45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{638C754D-6598-4F04-8D33-CB7A05B0560B}"/>
   </bookViews>
@@ -135,7 +135,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="341">
   <si>
     <t>Vehicle Data</t>
   </si>
@@ -299,9 +299,6 @@
     <t>Number of Cells</t>
   </si>
   <si>
-    <t>Model</t>
-  </si>
-  <si>
     <t>Regen Energy Generation</t>
   </si>
   <si>
@@ -771,9 +768,6 @@
   </si>
   <si>
     <t>Rated energy capacity of the battery</t>
-  </si>
-  <si>
-    <t>Battery model name/number</t>
   </si>
   <si>
     <t>State of Charge (SOC) at the start of the measurement period</t>
@@ -1611,10 +1605,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CA4D3C4-3E4D-4807-81BB-CD57E0DDC2A2}">
-  <dimension ref="A1:M156"/>
+  <dimension ref="A1:M155"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="C86" sqref="C86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1635,10 +1629,10 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="G1" s="2"/>
       <c r="I1" s="2"/>
@@ -1646,13 +1640,13 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="G2" s="2"/>
       <c r="I2" s="2"/>
@@ -1660,10 +1654,10 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C3" s="2"/>
       <c r="G3" s="2"/>
@@ -1672,10 +1666,10 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C4" s="2"/>
       <c r="G4" s="2"/>
@@ -1689,7 +1683,7 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="G6" s="2"/>
       <c r="I6" s="2"/>
@@ -1707,43 +1701,43 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="E9" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="F9" s="4" t="s">
+      <c r="G9" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="I9" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="G9" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="H9" s="4" t="s">
+      <c r="J9" s="4" t="s">
+        <v>340</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="M9" s="3" t="s">
         <v>104</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="J9" s="4" t="s">
-        <v>342</v>
-      </c>
-      <c r="K9" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="L9" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="M9" s="3" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -1755,7 +1749,7 @@
         <v>0</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -1764,10 +1758,10 @@
         <v>bev:battery_data</v>
       </c>
       <c r="C11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -1779,7 +1773,7 @@
         <v>45</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -1791,7 +1785,7 @@
         <v>3</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -1803,7 +1797,7 @@
         <v>2</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -1812,10 +1806,10 @@
         <v>bev:production_data</v>
       </c>
       <c r="C15" t="s">
+        <v>170</v>
+      </c>
+      <c r="F15" s="2" t="s">
         <v>171</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -1824,10 +1818,10 @@
         <v>bev:availability_kpis</v>
       </c>
       <c r="C16" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1836,10 +1830,10 @@
         <v>bev:utilization_kpis</v>
       </c>
       <c r="C17" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1848,10 +1842,10 @@
         <v>bev:effectiveness_kpis</v>
       </c>
       <c r="C18" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1860,10 +1854,10 @@
         <v>bev:maintenance_kpis</v>
       </c>
       <c r="C19" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -1875,10 +1869,10 @@
         <v>1</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -1890,10 +1884,10 @@
         <v>12</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J21" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -1905,10 +1899,10 @@
         <v>27</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J22" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -1923,7 +1917,7 @@
         <v>40</v>
       </c>
       <c r="J23" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -1938,7 +1932,7 @@
         <v>41</v>
       </c>
       <c r="J24" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1947,13 +1941,13 @@
         <v>bev:rebuild_count</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>42</v>
       </c>
       <c r="J25" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -1965,10 +1959,10 @@
         <v>43</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J26" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1980,10 +1974,10 @@
         <v>30</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J27" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -1995,10 +1989,10 @@
         <v>31</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="J28" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2007,13 +2001,13 @@
         <v>bev:functional_location</v>
       </c>
       <c r="C29" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="J29" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2022,16 +2016,16 @@
         <v>bev:energy_system_architecture</v>
       </c>
       <c r="C30" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="J30" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2040,16 +2034,16 @@
         <v>bev:vehicle_type</v>
       </c>
       <c r="C31" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="J31" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2061,13 +2055,13 @@
         <v>44</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="J32" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -2076,16 +2070,16 @@
         <v>bev:vehicle_function</v>
       </c>
       <c r="C33" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="J33" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -2097,10 +2091,10 @@
         <v>32</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J34" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -2109,16 +2103,16 @@
         <v>bev:gross_vehicle_weight</v>
       </c>
       <c r="C35" t="s">
+        <v>130</v>
+      </c>
+      <c r="F35" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F35" s="2" t="s">
-        <v>132</v>
-      </c>
       <c r="J35" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K35" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
@@ -2127,13 +2121,13 @@
         <v>bev:purchase_cost</v>
       </c>
       <c r="C36" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="J36" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -2145,10 +2139,10 @@
         <v>33</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J37" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -2160,10 +2154,10 @@
         <v>34</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J38" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -2175,10 +2169,10 @@
         <v>35</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J39" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
@@ -2190,10 +2184,10 @@
         <v>36</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J40" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -2202,16 +2196,16 @@
         <v>bev:auxiliary_powered_heater</v>
       </c>
       <c r="C41" t="s">
+        <v>105</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="J41" t="s">
         <v>106</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>325</v>
-      </c>
-      <c r="H41" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="J41" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -2223,10 +2217,10 @@
         <v>39</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J42" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="43" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -2235,16 +2229,16 @@
         <v>bev:charge_connector</v>
       </c>
       <c r="C43" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="J43" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -2253,13 +2247,13 @@
         <v>bev:measurement_start</v>
       </c>
       <c r="C44" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="J44" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="45" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -2268,13 +2262,13 @@
         <v>bev:measurement_end</v>
       </c>
       <c r="C45" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="J45" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="46" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -2283,13 +2277,13 @@
         <v>bev:vehicle_hours</v>
       </c>
       <c r="C46" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J46" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="47" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -2301,10 +2295,10 @@
         <v>11</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J47" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
@@ -2313,13 +2307,13 @@
         <v>bev:vehicle_idling_time</v>
       </c>
       <c r="C48" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J48" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
@@ -2331,10 +2325,10 @@
         <v>4</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J49" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
@@ -2346,10 +2340,10 @@
         <v>5</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J50" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
@@ -2358,13 +2352,13 @@
         <v>bev:queue_time</v>
       </c>
       <c r="C51" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J51" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
@@ -2373,13 +2367,13 @@
         <v>bev:battery_swapping_time</v>
       </c>
       <c r="C52" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J52" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2388,13 +2382,13 @@
         <v>bev:start_location</v>
       </c>
       <c r="C53" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J53" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2403,13 +2397,13 @@
         <v>bev:end_location</v>
       </c>
       <c r="C54" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J54" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="55" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2418,13 +2412,13 @@
         <v>bev:location</v>
       </c>
       <c r="C55" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="J55" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="56" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2436,10 +2430,10 @@
         <v>20</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J56" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
@@ -2448,13 +2442,13 @@
         <v>bev:speed</v>
       </c>
       <c r="C57" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J57" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
@@ -2463,13 +2457,13 @@
         <v>bev:acceleration</v>
       </c>
       <c r="C58" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J58" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="59" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2481,10 +2475,10 @@
         <v>47</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J59" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="60" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2496,10 +2490,10 @@
         <v>16</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J60" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="61" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2511,10 +2505,10 @@
         <v>9</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J61" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="62" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2526,10 +2520,10 @@
         <v>10</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J62" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
@@ -2541,10 +2535,10 @@
         <v>19</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J63" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
@@ -2553,13 +2547,13 @@
         <v>bev:hydraulic_system_energy</v>
       </c>
       <c r="C64" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J64" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2568,13 +2562,13 @@
         <v>bev:hydraulic_system_power</v>
       </c>
       <c r="C65" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J65" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="66" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2586,10 +2580,10 @@
         <v>17</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="J66" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="67" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2601,10 +2595,10 @@
         <v>18</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="J67" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
@@ -2613,13 +2607,13 @@
         <v>bev:payload</v>
       </c>
       <c r="C68" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J68" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2628,28 +2622,28 @@
         <v>bev:inclination</v>
       </c>
       <c r="C69" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J69" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" t="str">
-        <f t="shared" ref="A70:A136" si="3">CONCATENATE("bev:",LOWER(SUBSTITUTE(C70, " ", "_")))</f>
+        <f t="shared" ref="A70:A135" si="3">CONCATENATE("bev:",LOWER(SUBSTITUTE(C70, " ", "_")))</f>
         <v>bev:alert_id</v>
       </c>
       <c r="C70" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J70" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
@@ -2658,13 +2652,13 @@
         <v>bev:alert_type</v>
       </c>
       <c r="C71" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J71" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
@@ -2673,13 +2667,13 @@
         <v>bev:alert_description</v>
       </c>
       <c r="C72" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="J72" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
@@ -2688,13 +2682,13 @@
         <v>bev:alert_date_time</v>
       </c>
       <c r="C73" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="J73" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
@@ -2703,13 +2697,13 @@
         <v>bev:alert_status</v>
       </c>
       <c r="C74" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J74" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
@@ -2721,10 +2715,10 @@
         <v>12</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J75" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="76" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2733,13 +2727,13 @@
         <v>bev:pack_id</v>
       </c>
       <c r="C76" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J76" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
@@ -2751,10 +2745,10 @@
         <v>23</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="J77" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
@@ -2763,13 +2757,13 @@
         <v>bev:cell_id</v>
       </c>
       <c r="C78" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J78" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
@@ -2781,13 +2775,13 @@
         <v>37</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H79" s="2" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="J79" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
@@ -2799,10 +2793,10 @@
         <v>31</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J80" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
@@ -2814,10 +2808,10 @@
         <v>53</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="J81" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
@@ -2826,13 +2820,13 @@
         <v>bev:number_of_modules</v>
       </c>
       <c r="C82" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="J82" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="83" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -2841,13 +2835,13 @@
         <v>bev:number_of_packs</v>
       </c>
       <c r="C83" t="s">
+        <v>208</v>
+      </c>
+      <c r="F83" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="F83" s="2" t="s">
-        <v>210</v>
-      </c>
       <c r="J83" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
@@ -2859,448 +2853,448 @@
         <v>38</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="J84" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" t="str">
         <f t="shared" si="3"/>
-        <v>bev:model</v>
+        <v>bev:battery_mass</v>
       </c>
       <c r="C85" t="s">
-        <v>54</v>
+        <v>244</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>212</v>
+        <v>245</v>
       </c>
       <c r="J85" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A86" t="str">
         <f t="shared" si="3"/>
-        <v>bev:battery_mass</v>
+        <v>bev:initial_soc</v>
       </c>
       <c r="C86" t="s">
-        <v>246</v>
+        <v>6</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>247</v>
+        <v>211</v>
       </c>
       <c r="J86" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="87" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A87" t="str">
         <f t="shared" si="3"/>
-        <v>bev:initial_soc</v>
+        <v>bev:final_soc</v>
       </c>
       <c r="C87" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="J87" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="88" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A88" t="str">
-        <f t="shared" si="3"/>
-        <v>bev:final_soc</v>
+        <f>CONCATENATE("bev:",LOWER(SUBSTITUTE(C88, " ", "_")))</f>
+        <v>bev:soc</v>
       </c>
       <c r="C88" t="s">
-        <v>7</v>
+        <v>216</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>214</v>
+        <v>223</v>
       </c>
       <c r="J88" t="s">
-        <v>199</v>
+        <v>198</v>
+      </c>
+      <c r="K88" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="89" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A89" t="str">
-        <f>CONCATENATE("bev:",LOWER(SUBSTITUTE(C89, " ", "_")))</f>
-        <v>bev:soc</v>
+        <f t="shared" si="3"/>
+        <v>bev:soc_used</v>
       </c>
       <c r="C89" t="s">
+        <v>8</v>
+      </c>
+      <c r="F89" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="J89" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A90" t="str">
+        <f t="shared" si="3"/>
+        <v>bev:energy_consumption</v>
+      </c>
+      <c r="C90" t="s">
+        <v>214</v>
+      </c>
+      <c r="F90" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="J90" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A91" t="str">
+        <f t="shared" si="3"/>
+        <v>bev:regen_energy_generation</v>
+      </c>
+      <c r="C91" t="s">
+        <v>54</v>
+      </c>
+      <c r="F91" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="F89" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="J89" t="s">
-        <v>199</v>
-      </c>
-      <c r="K89" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="90" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A90" t="str">
-        <f t="shared" si="3"/>
-        <v>bev:soc_used</v>
-      </c>
-      <c r="C90" t="s">
-        <v>8</v>
-      </c>
-      <c r="F90" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="J90" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="91" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A91" t="str">
-        <f t="shared" si="3"/>
-        <v>bev:energy_consumption</v>
-      </c>
-      <c r="C91" t="s">
-        <v>216</v>
-      </c>
-      <c r="F91" s="2" t="s">
-        <v>219</v>
-      </c>
       <c r="J91" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="92" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A92" t="str">
         <f t="shared" si="3"/>
-        <v>bev:regen_energy_generation</v>
+        <v>bev:net_energy_consumption</v>
       </c>
       <c r="C92" t="s">
-        <v>55</v>
+        <v>215</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="J92" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="93" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A93" t="str">
         <f t="shared" si="3"/>
-        <v>bev:net_energy_consumption</v>
+        <v>bev:average_battery_voltage</v>
       </c>
       <c r="C93" t="s">
-        <v>217</v>
+        <v>21</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="J93" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="94" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A94" t="str">
         <f t="shared" si="3"/>
-        <v>bev:average_battery_voltage</v>
+        <v>bev:average_battery_current</v>
       </c>
       <c r="C94" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F94" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="J94" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A95" t="str">
+        <f t="shared" si="3"/>
+        <v>bev:battery_voltage</v>
+      </c>
+      <c r="C95" t="s">
+        <v>24</v>
+      </c>
+      <c r="F95" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="J94" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="95" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A95" t="str">
-        <f t="shared" si="3"/>
-        <v>bev:average_battery_current</v>
-      </c>
-      <c r="C95" t="s">
-        <v>22</v>
-      </c>
-      <c r="F95" s="2" t="s">
-        <v>223</v>
-      </c>
       <c r="J95" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" t="str">
         <f t="shared" si="3"/>
-        <v>bev:battery_voltage</v>
+        <v>bev:battery_power</v>
       </c>
       <c r="C96" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F96" s="2" t="s">
         <v>224</v>
       </c>
       <c r="J96" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" t="str">
         <f t="shared" si="3"/>
-        <v>bev:battery_power</v>
+        <v>bev:battery_current</v>
       </c>
       <c r="C97" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="J97" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" t="str">
         <f t="shared" si="3"/>
-        <v>bev:battery_current</v>
+        <v>bev:battery_temperature</v>
       </c>
       <c r="C98" t="s">
-        <v>26</v>
+        <v>75</v>
       </c>
       <c r="F98" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="J98" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A99" t="str">
+        <f t="shared" si="3"/>
+        <v>bev:soh</v>
+      </c>
+      <c r="C99" t="s">
+        <v>74</v>
+      </c>
+      <c r="F99" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="J98" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A99" t="str">
-        <f t="shared" si="3"/>
-        <v>bev:battery_temperature</v>
-      </c>
-      <c r="C99" t="s">
-        <v>76</v>
-      </c>
-      <c r="F99" s="2" t="s">
+      <c r="J99" t="s">
+        <v>198</v>
+      </c>
+      <c r="K99" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A100" t="str">
+        <f t="shared" si="3"/>
+        <v>bev:charger_id</v>
+      </c>
+      <c r="C100" t="s">
+        <v>46</v>
+      </c>
+      <c r="F100" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="J100" t="s">
         <v>228</v>
-      </c>
-      <c r="J99" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="100" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A100" t="str">
-        <f t="shared" si="3"/>
-        <v>bev:soh</v>
-      </c>
-      <c r="C100" t="s">
-        <v>75</v>
-      </c>
-      <c r="F100" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="J100" t="s">
-        <v>199</v>
-      </c>
-      <c r="K100" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" t="str">
         <f t="shared" si="3"/>
-        <v>bev:charger_id</v>
+        <v>bev:connector_id</v>
       </c>
       <c r="C101" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="F101" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="J101" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A102" t="str">
-        <f t="shared" si="3"/>
-        <v>bev:connector_id</v>
+        <f>CONCATENATE("bev:",LOWER(SUBSTITUTE(C102, " ", "_")))</f>
+        <v>bev:max_power</v>
       </c>
       <c r="C102" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="F102" s="2" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="J102" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="103" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" t="str">
         <f>CONCATENATE("bev:",LOWER(SUBSTITUTE(C103, " ", "_")))</f>
-        <v>bev:max_power</v>
+        <v>bev:rated_power</v>
       </c>
       <c r="C103" t="s">
-        <v>49</v>
+        <v>237</v>
       </c>
       <c r="F103" s="2" t="s">
         <v>238</v>
       </c>
       <c r="J103" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A104" t="str">
         <f>CONCATENATE("bev:",LOWER(SUBSTITUTE(C104, " ", "_")))</f>
-        <v>bev:rated_power</v>
+        <v>bev:charger_location</v>
       </c>
       <c r="C104" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="J104" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="105" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A105" t="str">
         <f>CONCATENATE("bev:",LOWER(SUBSTITUTE(C105, " ", "_")))</f>
-        <v>bev:charger_location</v>
+        <v>bev:charge_start_time</v>
       </c>
       <c r="C105" t="s">
-        <v>243</v>
+        <v>51</v>
       </c>
       <c r="F105" s="2" t="s">
-        <v>244</v>
+        <v>232</v>
       </c>
       <c r="J105" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="106" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A106" t="str">
         <f>CONCATENATE("bev:",LOWER(SUBSTITUTE(C106, " ", "_")))</f>
-        <v>bev:charge_start_time</v>
+        <v>bev:charge_end_time</v>
       </c>
       <c r="C106" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>234</v>
+        <v>240</v>
       </c>
       <c r="J106" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="107" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" t="str">
-        <f>CONCATENATE("bev:",LOWER(SUBSTITUTE(C107, " ", "_")))</f>
-        <v>bev:charge_end_time</v>
+        <f t="shared" si="3"/>
+        <v>bev:charging_time</v>
       </c>
       <c r="C107" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="J107" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" t="str">
         <f t="shared" si="3"/>
-        <v>bev:charging_time</v>
+        <v>bev:charging_power</v>
       </c>
       <c r="C108" t="s">
-        <v>48</v>
+        <v>234</v>
       </c>
       <c r="F108" s="2" t="s">
         <v>235</v>
       </c>
       <c r="J108" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" t="str">
         <f t="shared" si="3"/>
-        <v>bev:charging_power</v>
+        <v>bev:charging_rate</v>
       </c>
       <c r="C109" t="s">
-        <v>236</v>
+        <v>314</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>237</v>
+        <v>329</v>
+      </c>
+      <c r="H109" s="2" t="s">
+        <v>328</v>
       </c>
       <c r="J109" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+        <v>228</v>
+      </c>
+      <c r="K109" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A110" t="str">
         <f t="shared" si="3"/>
-        <v>bev:charging_rate</v>
+        <v>bev:total_energy_delivered</v>
       </c>
       <c r="C110" t="s">
-        <v>316</v>
+        <v>50</v>
       </c>
       <c r="F110" s="2" t="s">
-        <v>331</v>
-      </c>
-      <c r="H110" s="2" t="s">
-        <v>330</v>
+        <v>239</v>
       </c>
       <c r="J110" t="s">
-        <v>230</v>
-      </c>
-      <c r="K110" t="s">
-        <v>317</v>
+        <v>228</v>
       </c>
     </row>
     <row r="111" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A111" t="str">
         <f t="shared" si="3"/>
-        <v>bev:total_energy_delivered</v>
+        <v>bev:work_order_id</v>
       </c>
       <c r="C111" t="s">
-        <v>50</v>
+        <v>115</v>
       </c>
       <c r="F111" s="2" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="J111" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="112" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" t="str">
         <f t="shared" si="3"/>
-        <v>bev:work_order_id</v>
+        <v>bev:work_order_description</v>
       </c>
       <c r="C112" t="s">
-        <v>116</v>
+        <v>250</v>
       </c>
       <c r="F112" s="2" t="s">
         <v>251</v>
       </c>
       <c r="J112" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113" t="str">
         <f t="shared" si="3"/>
-        <v>bev:work_order_description</v>
+        <v>bev:work_order_status</v>
       </c>
       <c r="C113" t="s">
         <v>252</v>
@@ -3309,193 +3303,196 @@
         <v>253</v>
       </c>
       <c r="J113" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="114" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A114" t="str">
         <f t="shared" si="3"/>
-        <v>bev:work_order_status</v>
+        <v>bev:technician_name</v>
       </c>
       <c r="C114" t="s">
+        <v>58</v>
+      </c>
+      <c r="F114" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="F114" s="2" t="s">
+      <c r="J114" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A115" t="str">
+        <f t="shared" si="3"/>
+        <v>bev:work_order_type</v>
+      </c>
+      <c r="C115" t="s">
+        <v>60</v>
+      </c>
+      <c r="F115" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="J114" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="115" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A115" t="str">
-        <f t="shared" si="3"/>
-        <v>bev:technician_name</v>
-      </c>
-      <c r="C115" t="s">
-        <v>59</v>
-      </c>
-      <c r="F115" s="2" t="s">
-        <v>256</v>
-      </c>
       <c r="J115" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116" t="str">
         <f t="shared" si="3"/>
-        <v>bev:work_order_type</v>
+        <v>bev:priority</v>
       </c>
       <c r="C116" t="s">
         <v>61</v>
       </c>
       <c r="F116" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="J116" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A117" t="str">
+        <f t="shared" si="3"/>
+        <v>bev:work_center</v>
+      </c>
+      <c r="C117" t="s">
+        <v>59</v>
+      </c>
+      <c r="F117" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="J116" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A117" t="str">
-        <f t="shared" si="3"/>
-        <v>bev:priority</v>
-      </c>
-      <c r="C117" t="s">
-        <v>62</v>
-      </c>
-      <c r="F117" s="2" t="s">
+      <c r="J117" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A118" t="str">
+        <f t="shared" si="3"/>
+        <v>bev:work_order_start</v>
+      </c>
+      <c r="C118" t="s">
         <v>258</v>
       </c>
-      <c r="J117" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="118" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A118" t="str">
-        <f t="shared" si="3"/>
-        <v>bev:work_center</v>
-      </c>
-      <c r="C118" t="s">
-        <v>60</v>
-      </c>
       <c r="F118" s="2" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="J118" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A119" t="str">
         <f t="shared" si="3"/>
-        <v>bev:work_order_start</v>
+        <v>bev:work_order_end</v>
       </c>
       <c r="C119" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F119" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="J119" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120" t="str">
         <f t="shared" si="3"/>
-        <v>bev:work_order_end</v>
+        <v>bev:total_costs</v>
       </c>
       <c r="C120" t="s">
-        <v>261</v>
+        <v>62</v>
       </c>
       <c r="F120" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J120" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A121" t="str">
         <f t="shared" si="3"/>
-        <v>bev:total_costs</v>
+        <v>bev:part_costs</v>
       </c>
       <c r="C121" t="s">
-        <v>63</v>
+        <v>116</v>
       </c>
       <c r="F121" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="J121" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122" t="str">
         <f t="shared" si="3"/>
-        <v>bev:part_costs</v>
+        <v>bev:labour_costs</v>
       </c>
       <c r="C122" t="s">
         <v>117</v>
       </c>
       <c r="F122" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="J122" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123" t="str">
         <f t="shared" si="3"/>
-        <v>bev:labour_costs</v>
+        <v>bev:time_in_workshop</v>
       </c>
       <c r="C123" t="s">
-        <v>118</v>
+        <v>192</v>
       </c>
       <c r="F123" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="J123" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="124" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A124" t="str">
         <f t="shared" si="3"/>
-        <v>bev:time_in_workshop</v>
+        <v>bev:logistic_delay</v>
       </c>
       <c r="C124" t="s">
         <v>193</v>
       </c>
       <c r="F124" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="J124" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="125" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A125" t="str">
         <f t="shared" si="3"/>
-        <v>bev:logistic_delay</v>
+        <v>bev:time_to_repair</v>
       </c>
       <c r="C125" t="s">
         <v>194</v>
       </c>
       <c r="F125" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="J125" t="s">
-        <v>245</v>
+        <v>243</v>
+      </c>
+      <c r="K125" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A126" t="str">
         <f t="shared" si="3"/>
-        <v>bev:time_to_repair</v>
+        <v>bev:idle_time</v>
       </c>
       <c r="C126" t="s">
         <v>195</v>
@@ -3504,484 +3501,466 @@
         <v>269</v>
       </c>
       <c r="J126" t="s">
-        <v>245</v>
-      </c>
-      <c r="K126" t="s">
-        <v>313</v>
+        <v>243</v>
       </c>
     </row>
     <row r="127" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A127" t="str">
         <f t="shared" si="3"/>
-        <v>bev:idle_time</v>
+        <v>bev:mean_time_to_repair</v>
       </c>
       <c r="C127" t="s">
-        <v>196</v>
+        <v>86</v>
       </c>
       <c r="F127" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="J127" t="s">
-        <v>245</v>
+        <v>336</v>
+      </c>
+      <c r="K127" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="128" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A128" t="str">
         <f t="shared" si="3"/>
-        <v>bev:mean_time_to_repair</v>
+        <v>bev:mean_time_between_failures</v>
       </c>
       <c r="C128" t="s">
-        <v>87</v>
+        <v>196</v>
       </c>
       <c r="F128" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="J128" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="K128" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="129" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A129" t="str">
         <f t="shared" si="3"/>
-        <v>bev:mean_time_between_failures</v>
+        <v>bev:mean_time_between_maintenance</v>
       </c>
       <c r="C129" t="s">
-        <v>197</v>
+        <v>65</v>
       </c>
       <c r="F129" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="J129" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="K129" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="130" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A130" t="str">
         <f t="shared" si="3"/>
-        <v>bev:mean_time_between_maintenance</v>
+        <v>bev:mean_down_time</v>
       </c>
       <c r="C130" t="s">
-        <v>66</v>
+        <v>197</v>
       </c>
       <c r="F130" s="2" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="J130" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="K130" t="s">
-        <v>15</v>
+        <v>83</v>
       </c>
     </row>
     <row r="131" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A131" t="str">
         <f t="shared" si="3"/>
-        <v>bev:mean_down_time</v>
+        <v>bev:calendar_time</v>
       </c>
       <c r="C131" t="s">
-        <v>198</v>
+        <v>172</v>
       </c>
       <c r="F131" s="2" t="s">
-        <v>270</v>
+        <v>276</v>
       </c>
       <c r="J131" t="s">
-        <v>338</v>
-      </c>
-      <c r="K131" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="132" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A132" t="str">
         <f t="shared" si="3"/>
-        <v>bev:calendar_time</v>
+        <v>bev:scheduled_time</v>
       </c>
       <c r="C132" t="s">
         <v>173</v>
       </c>
       <c r="F132" s="2" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="J132" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="133" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A133" t="str">
-        <f t="shared" si="3"/>
-        <v>bev:scheduled_time</v>
+        <f>CONCATENATE("bev:",LOWER(SUBSTITUTE(C133, " ", "_")))</f>
+        <v>bev:unscheduled_time</v>
       </c>
       <c r="C133" t="s">
-        <v>174</v>
+        <v>188</v>
       </c>
       <c r="F133" s="2" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="J133" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="134" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A134" t="str">
         <f>CONCATENATE("bev:",LOWER(SUBSTITUTE(C134, " ", "_")))</f>
-        <v>bev:unscheduled_time</v>
+        <v>bev:down_time</v>
       </c>
       <c r="C134" t="s">
-        <v>189</v>
+        <v>274</v>
       </c>
       <c r="F134" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="J134" t="s">
+        <v>273</v>
+      </c>
+      <c r="K134" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="135" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A135" t="str">
+        <f t="shared" si="3"/>
+        <v>bev:available_time</v>
+      </c>
+      <c r="C135" t="s">
+        <v>174</v>
+      </c>
+      <c r="F135" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="J134" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="135" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A135" t="str">
-        <f>CONCATENATE("bev:",LOWER(SUBSTITUTE(C135, " ", "_")))</f>
-        <v>bev:down_time</v>
-      </c>
-      <c r="C135" t="s">
-        <v>276</v>
-      </c>
-      <c r="F135" s="2" t="s">
-        <v>280</v>
-      </c>
       <c r="J135" t="s">
-        <v>275</v>
-      </c>
-      <c r="K135" t="s">
-        <v>314</v>
+        <v>273</v>
       </c>
     </row>
     <row r="136" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A136" t="str">
-        <f t="shared" si="3"/>
-        <v>bev:available_time</v>
+        <f>CONCATENATE("bev:",LOWER(SUBSTITUTE(C136, " ", "_")))</f>
+        <v>bev:standby_time</v>
       </c>
       <c r="C136" t="s">
-        <v>175</v>
+        <v>189</v>
       </c>
       <c r="F136" s="2" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="J136" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="137" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="137" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A137" t="str">
         <f>CONCATENATE("bev:",LOWER(SUBSTITUTE(C137, " ", "_")))</f>
-        <v>bev:standby_time</v>
+        <v>bev:operating_standby_time</v>
       </c>
       <c r="C137" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
       <c r="F137" s="2" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="J137" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="138" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A138" t="str">
         <f>CONCATENATE("bev:",LOWER(SUBSTITUTE(C138, " ", "_")))</f>
-        <v>bev:operating_standby_time</v>
+        <v>bev:external_standby_time</v>
       </c>
       <c r="C138" t="s">
         <v>179</v>
       </c>
       <c r="F138" s="2" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="J138" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="139" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="139" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A139" t="str">
-        <f>CONCATENATE("bev:",LOWER(SUBSTITUTE(C139, " ", "_")))</f>
-        <v>bev:external_standby_time</v>
+        <f t="shared" ref="A139:A155" si="4">CONCATENATE("bev:",LOWER(SUBSTITUTE(C139, " ", "_")))</f>
+        <v>bev:operating_time</v>
       </c>
       <c r="C139" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="F139" s="2" t="s">
         <v>283</v>
       </c>
       <c r="J139" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="140" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="140" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A140" t="str">
-        <f t="shared" ref="A140:A156" si="4">CONCATENATE("bev:",LOWER(SUBSTITUTE(C140, " ", "_")))</f>
-        <v>bev:operating_time</v>
+        <f>CONCATENATE("bev:",LOWER(SUBSTITUTE(C140, " ", "_")))</f>
+        <v>bev:operating_delay</v>
       </c>
       <c r="C140" t="s">
-        <v>176</v>
+        <v>190</v>
       </c>
       <c r="F140" s="2" t="s">
         <v>285</v>
       </c>
       <c r="J140" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="141" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="141" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A141" t="str">
-        <f>CONCATENATE("bev:",LOWER(SUBSTITUTE(C141, " ", "_")))</f>
-        <v>bev:operating_delay</v>
-      </c>
-      <c r="C141" t="s">
-        <v>191</v>
-      </c>
-      <c r="F141" s="2" t="s">
-        <v>287</v>
-      </c>
-      <c r="J141" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="142" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A142" t="str">
         <f t="shared" si="4"/>
         <v>bev:working_time</v>
       </c>
+      <c r="C141" t="s">
+        <v>176</v>
+      </c>
+      <c r="F141" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="J141" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="142" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A142" t="str">
+        <f>CONCATENATE("bev:",LOWER(SUBSTITUTE(C142, " ", "_")))</f>
+        <v>bev:non-productive_time</v>
+      </c>
       <c r="C142" t="s">
+        <v>191</v>
+      </c>
+      <c r="F142" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="J142" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="143" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A143" t="str">
+        <f t="shared" si="4"/>
+        <v>bev:productive_time</v>
+      </c>
+      <c r="C143" t="s">
         <v>177</v>
       </c>
-      <c r="F142" s="2" t="s">
+      <c r="F143" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="J142" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="143" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A143" t="str">
-        <f>CONCATENATE("bev:",LOWER(SUBSTITUTE(C143, " ", "_")))</f>
-        <v>bev:non-productive_time</v>
-      </c>
-      <c r="C143" t="s">
-        <v>192</v>
-      </c>
-      <c r="F143" s="2" t="s">
-        <v>289</v>
-      </c>
       <c r="J143" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="144" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="144" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A144" t="str">
         <f t="shared" si="4"/>
-        <v>bev:productive_time</v>
+        <v>bev:up_time</v>
       </c>
       <c r="C144" t="s">
-        <v>178</v>
+        <v>275</v>
       </c>
       <c r="F144" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="J144" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="145" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>337</v>
+      </c>
+      <c r="K144" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="145" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A145" t="str">
         <f t="shared" si="4"/>
-        <v>bev:up_time</v>
+        <v>bev:availability</v>
       </c>
       <c r="C145" t="s">
-        <v>277</v>
+        <v>290</v>
       </c>
       <c r="F145" s="2" t="s">
-        <v>291</v>
+        <v>309</v>
       </c>
       <c r="J145" t="s">
-        <v>339</v>
-      </c>
-      <c r="K145" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="146" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="146" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A146" t="str">
         <f t="shared" si="4"/>
-        <v>bev:availability</v>
+        <v>bev:physical_availability</v>
       </c>
       <c r="C146" t="s">
-        <v>292</v>
+        <v>180</v>
       </c>
       <c r="F146" s="2" t="s">
-        <v>311</v>
+        <v>291</v>
       </c>
       <c r="J146" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="147" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="147" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A147" t="str">
         <f t="shared" si="4"/>
-        <v>bev:physical_availability</v>
+        <v>bev:mechanical_availability</v>
       </c>
       <c r="C147" t="s">
         <v>181</v>
       </c>
       <c r="F147" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="J147" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="148" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A148" t="str">
         <f t="shared" si="4"/>
-        <v>bev:mechanical_availability</v>
+        <v>bev:use_of_availability</v>
       </c>
       <c r="C148" t="s">
         <v>182</v>
       </c>
       <c r="F148" s="2" t="s">
-        <v>294</v>
+        <v>301</v>
       </c>
       <c r="J148" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="149" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A149" t="str">
         <f t="shared" si="4"/>
-        <v>bev:use_of_availability</v>
+        <v>bev:asset_utilization</v>
       </c>
       <c r="C149" t="s">
         <v>183</v>
       </c>
       <c r="F149" s="2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="J149" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="150" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A150" t="str">
         <f t="shared" si="4"/>
-        <v>bev:asset_utilization</v>
+        <v>bev:operating_utilization</v>
       </c>
       <c r="C150" t="s">
         <v>184</v>
       </c>
       <c r="F150" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="J150" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="151" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="151" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A151" t="str">
         <f t="shared" si="4"/>
-        <v>bev:operating_utilization</v>
+        <v>bev:effective_utilization</v>
       </c>
       <c r="C151" t="s">
         <v>185</v>
       </c>
       <c r="F151" s="2" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="J151" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="152" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A152" t="str">
         <f t="shared" si="4"/>
-        <v>bev:effective_utilization</v>
+        <v>bev:operating_efficiency</v>
       </c>
       <c r="C152" t="s">
         <v>186</v>
       </c>
       <c r="F152" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="J152" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="153" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A153" t="str">
         <f t="shared" si="4"/>
-        <v>bev:operating_efficiency</v>
+        <v>bev:production_effectiveness</v>
       </c>
       <c r="C153" t="s">
         <v>187</v>
       </c>
       <c r="F153" s="2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="J153" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="154" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A154" t="str">
-        <f t="shared" si="4"/>
-        <v>bev:production_effectiveness</v>
+        <f>CONCATENATE("bev:",LOWER(SUBSTITUTE(C154, " ", "_")))</f>
+        <v>bev:overall_equipment_effectiveness</v>
       </c>
       <c r="C154" t="s">
-        <v>188</v>
+        <v>88</v>
       </c>
       <c r="F154" s="2" t="s">
         <v>308</v>
       </c>
       <c r="J154" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="155" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+        <v>339</v>
+      </c>
+      <c r="K154" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="155" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A155" t="str">
-        <f>CONCATENATE("bev:",LOWER(SUBSTITUTE(C155, " ", "_")))</f>
-        <v>bev:overall_equipment_effectiveness</v>
-      </c>
-      <c r="C155" t="s">
-        <v>89</v>
-      </c>
-      <c r="F155" s="2" t="s">
-        <v>310</v>
-      </c>
-      <c r="J155" t="s">
-        <v>341</v>
-      </c>
-      <c r="K155" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="156" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A156" t="str">
         <f t="shared" si="4"/>
         <v>bev:mean_operating_time</v>
       </c>
-      <c r="C156" t="s">
-        <v>86</v>
-      </c>
-      <c r="F156" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="J156" t="s">
-        <v>275</v>
-      </c>
-      <c r="K156" t="s">
+      <c r="C155" t="s">
         <v>85</v>
+      </c>
+      <c r="F155" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="J155" t="s">
+        <v>273</v>
+      </c>
+      <c r="K155" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -3991,12 +3970,13 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d8e165db-149b-4197-bc76-0f068cbb73e1">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4211,19 +4191,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d8e165db-149b-4197-bc76-0f068cbb73e1">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B902C61F-C425-480E-9AE8-5743FFC97C42}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0058CAD2-89AE-44C8-AF19-A0D04C3633AC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="d8e165db-149b-4197-bc76-0f068cbb73e1"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4248,11 +4229,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0058CAD2-89AE-44C8-AF19-A0D04C3633AC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B902C61F-C425-480E-9AE8-5743FFC97C42}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="d8e165db-149b-4197-bc76-0f068cbb73e1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Created example data seed json
</commit_message>
<xml_diff>
--- a/BEV Data Vocabulary.xlsx
+++ b/BEV Data Vocabulary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edwar\Github\evmo-vocab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CC1F5B6-F0F0-49EE-B0AF-ADE7BF219E45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC26B0CF-87AB-4F75-98B1-418B24CD1BD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{638C754D-6598-4F04-8D33-CB7A05B0560B}"/>
   </bookViews>
@@ -1607,8 +1607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CA4D3C4-3E4D-4807-81BB-CD57E0DDC2A2}">
   <dimension ref="A1:M155"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="C86" sqref="C86"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1616,11 +1616,11 @@
     <col min="1" max="1" width="30.140625" customWidth="1"/>
     <col min="2" max="2" width="16.7109375" customWidth="1"/>
     <col min="3" max="3" width="30.5703125" customWidth="1"/>
-    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="48.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" customWidth="1"/>
     <col min="6" max="6" width="33" style="2" customWidth="1"/>
     <col min="7" max="7" width="28" customWidth="1"/>
-    <col min="8" max="8" width="28" style="2" customWidth="1"/>
+    <col min="8" max="8" width="46.140625" style="2" customWidth="1"/>
     <col min="9" max="9" width="28" customWidth="1"/>
     <col min="10" max="10" width="48.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="28" customWidth="1"/>
@@ -2010,7 +2010,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
         <f t="shared" si="1"/>
         <v>bev:energy_system_architecture</v>
@@ -3970,13 +3970,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d8e165db-149b-4197-bc76-0f068cbb73e1">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4191,20 +4190,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d8e165db-149b-4197-bc76-0f068cbb73e1">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0058CAD2-89AE-44C8-AF19-A0D04C3633AC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B902C61F-C425-480E-9AE8-5743FFC97C42}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="d8e165db-149b-4197-bc76-0f068cbb73e1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4229,9 +4227,11 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B902C61F-C425-480E-9AE8-5743FFC97C42}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0058CAD2-89AE-44C8-AF19-A0D04C3633AC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="d8e165db-149b-4197-bc76-0f068cbb73e1"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>